<commit_message>
Get daily reddit data: Tue Jul 22 08:14:22 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_07_27.xlsx
+++ b/data/collected_data/2025_07_27.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C510"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,3559 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1m681th</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Neutral but nice!</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/i1j4xw3psdef1</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1m67xrj</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Am I doing this cateye thing right?</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m67xrj</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1m67rn5</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Late night nails ft. Muffin the kitty ❣️ Advice on making sure they last?</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m67rn5/late_night_nails_ft_muffin_the_kitty_advice_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1m67kvj</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Rate my friend's nails</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m67kvj</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1m67aj1</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Very long for me, but I love my new set of claws 🖤🔮🐈‍⬛</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xlhcrmszjdef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1m66xb9</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Lastest press on nail set I made</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rp1zpqptfdef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1m66r65</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Hate my new nails but figured I’d post them anywho :’D</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tm7y675xddef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1m66pbj</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>Gel x diy</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m66pbj</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1m66aci</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>Is there any way to make my nail beds grow longer?</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m3n63wrn8def1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1m65ejf</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>Going to an Indy race so I decided to get the flags for my current set!</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wqv9v689zcef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1m65edm</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Blueberries</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vmkgovp6zcef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1m65dgi</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Has anyone tried these translucent chrome powders? Or have any recommendations?</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m65dgi</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1m658y4</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>finished these cuties today!</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m658y4</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1m64xd4</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Looking for advice re base coat please</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m64xd4/looking_for_advice_re_base_coat_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1m64t6s</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>I got my nails done for the first time!!!! (Gel-paint)</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m64t6s</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1m63zxc</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>One of my fave sets I’ve done in a long time!!</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m63zxc</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1m6481l</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>I’m a nail hobbyist and this is my first time installing gel tips (fakes lol)!</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3m3swcooncef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1m643zj</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>My nails these last 5 months</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m643zj</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1m63w4h</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>💫✨</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m63w4h</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1m63lzb</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>Went to Alaska and got mountain nails!</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jm2cl2vzhcef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1m63gki</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>Vacay Nails</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rde8l27kgcef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1m63ghw</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>This!!</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m63ghw</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1m63a7z</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Gel nail polish destroyed my nails</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m63a7z/gel_nail_polish_destroyed_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1m61fws</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>Witchy vibes</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m61fws</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1m61wz9</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>What DO you recommend?</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m61wz9/what_do_you_recommend/</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1m62spk</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Love! Super subtle and the deco gives it the special touch ✨️</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u2yiis6sacef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1m61xpy</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Some of my fav Halloween nails I’ve had! 🎃</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bg9j1mtc3cef1</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1m61im7</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Picnic Time! 🧺🍓🏵️</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m61im7</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1m61dki</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Guava drops 🥝 🍉</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cyenur8mybef1</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1m60u84</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Fresh new trash pandas 🥰</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lsohxpo0ubef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1m60tci</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>This is a long shot but what could be causing this UV glow? textureless, odorless, and completely invisible without UV light</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m60tci</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1m60cry</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>Made my first set of press-ons!</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7go22y2xpbef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1m5zzib</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>New set!!</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5zzib</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1m5zw2d</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Love love love my new nail tech</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/48mquwuzlbef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1m5zr3d</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Taking a break from acrylics</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5zr3d</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1m5zfnn</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>How to take care of press on nails.</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m5zfnn/how_to_take_care_of_press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1m5zgc4</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>What do I ask for if I want this?</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r4wmgumdibef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1m5ycrp</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Help me find this color!</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/83fvnm9l9bef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1m5yn1e</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>I had my first client that wasn’t a family member or a friend today!</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5yn1e</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1m5qom6</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Help! Broken natural nail under dip manicure</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xv9vcd24r9ef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1m5sthz</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Tips and Tricks for how to remove semi-cured gel strips?</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m5sthz/tips_and_tricks_for_how_to_remove_semicured_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1m5xds3</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Painted my nails today! Inspired by the BBC3 TV show Fleabag</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/twjftjn72bef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1m5xumw</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Do you guys have a soft gel brand recommendation?</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m5xumw/do_you_guys_have_a_soft_gel_brand_recommendation/</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1m5xksy</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>how to take them off?</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/53pm1v0p3bef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1m5w7oc</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>First time nails!</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1d76is9qtaef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1m5wtgr</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Getting some practice in</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5wtgr</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1m5x96k</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>how can i soften up my sharp nails?</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pdi9dt3a1bef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1m5vwlw</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>New nails!</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5vwlw</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1m5x0rd</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Frenchies with white chrome 🤍</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bzabqjnjzaef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1m5w11b</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>butterfly wings!!!</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5w11b</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1m5vqil</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>Cat Eye 💅</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8dpz7r5cqaef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1m5vip3</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>Is this actually good?</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m5vip3/is_this_actually_good/</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1m5us1q</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>Textured Glass Nails 😍 pictures don't do this one justice</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5us1q</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1m5ulff</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Every single good r/nails post gets locked, can we not be weird to women with hands!?! (Image unrelated)</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ef5oz5ogiaef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1m5ugsq</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>Good enough?</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u04mz3wkhaef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1m5togw</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>First time using acrylic!!</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/aevw6ujacaef1</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1m5u4wn</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>Internship nails</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5u4wn</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1m5tu98</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>3D Gel Nail Art 🐛</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5tu98</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1m5tphk</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>made my friend's nails!</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5tphk</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1m5tokq</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>charming manicure with coating</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r3dz3e6ccaef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1m5tkt1</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>Sally Hansen - hard drive me crazy</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5tkt1</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1m5tjcq</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>summer nails</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5tjcq</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1m5tas1</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>Mango nails</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nkda70us9aef1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1m5t843</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>Tips for growing out weak nails?</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zrchbmra9aef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1m5t7bj</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>Today's work</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a5n4hrf59aef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1m5syxh</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>Is this all I need to start making  nails?</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m5syxh/is_this_all_i_need_to_start_making_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1m5sk9j</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>My client wanted Beyoncé cowboy carter nails so I took on the challenge !</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9l5dz33s4aef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1m5s9k1</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Pretty nails</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2v1jcj1t2aef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1m5s5rd</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>bunch of people thought i couldn't wash my hair do dishes etc. so here's a little demo of how i pull the chain taut!!</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5s5rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1m5ruhf</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>Birthday Nail Set!</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vapma9z00aef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1m5rpwn</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>Natural nails are finally growing out… first time they’ve ever been this long and not broken</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/blce64l6z9ef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1m5r6qd</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>The final boss of rings of fire..</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5r6qd</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1m5qwl7</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>So proud of how this set came out! Hope they last 👀</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5qwl7</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1m5qr1n</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>When The Cat Eye Hits Just Right - Nikki Nailed it</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/168ilp6qs9ef1</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1m5qnzn</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Summer fruit appreciation</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5qnzn</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1m5qkrt</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>Did these myself</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5qkrt</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1m5qk56</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>Summer🤍</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mp32vlhgr9ef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1m5qads</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>have my nails improved a tiny bit 😔😔 (i unfortunately am a chronic nail biter but i just bought the bite nail polish so hopefully that helps)</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5qads</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1m5pyut</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>Clase Azul Tequila inspired nails for my Mexico trip!</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5pyut</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1m5pxwb</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>Poor brush</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1njt1zldn9ef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1m5ppba</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>I like how the new nails I made turned out!</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sxhntp1ol9ef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1m5po77</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Earlier I saw someone post their gamer girly nails and I want to jump in this too &lt;3</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qf3rb7qll9ef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1m5p85k</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Nail art question</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m5p85k/nail_art_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1m5mb7x</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>My nail bed split in half when soaking off my acrylics, what do i do?</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/232ebjiiz8ef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1m50dub</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>Allergy to gel?</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gdyk43vii3ef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1m55d7a</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Help</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m55d7a</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1m5ojgp</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Recommendations after experiencing allergies</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m5ojgp/recommendations_after_experiencing_allergies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1m5obds</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Thoughts on this color? 💅</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5obds</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1m5omhh</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>my first manicure. brown jelly nails gurl😙</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/im34zrqte9ef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1m5ogvm</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Atomic Nails- Sour Apple Rings</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mps25bwtd9ef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1m5oglh</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>Cats eye</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/llhutl6sd9ef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1m5ofnq</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>My first nail polish 💅</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ehzesomd9ef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1m5ocp1</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>Did they do a good job?</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iyo0vf23d9ef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1m5o766</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>Floral summer multicolor French tips</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5o766</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1m5o43n</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>My latest (gel on natural nails)</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/meq40zajb9ef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1m5ntx4</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Chrome is so pretty</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/muegg76o99ef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1m5nrre</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>Chinese nails</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/eupbb73a99ef1</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1m5nih3</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Do these look bad?</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gybcl3bj79ef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1m5ne1m</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Angular Nail Bed (Thumbs)</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5ne1m</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1m5ndk8</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>When I need a little reminder...</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5ndk8</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1m686ut</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Some of my 2025 manicures</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m686ut</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1m685wg</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>broken nail when getting nails removed? help!</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m685wg</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1m66zwp</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>I think my nail tech lied about the product?</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m66zwp/i_think_my_nail_tech_lied_about_the_product/</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1m65jaz</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>🔮🌕🧌BKL Swamp Witch Summer 🧌🌕🔮</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m65jaz</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1m65bs2</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Can't Stop Staring At My Nails</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m65bs2</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1m6504s</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>i need polish in this hot sauce color!! help! its so hot and im obsessed</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yc99r4i9vcef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1m64uxq</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>✨ She’s headed straight for the castle… with claws forged in gemstone ✨</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m64uxq</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1m64jfc</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>night sky nail polish recommendations</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m64jfc/night_sky_nail_polish_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1m64f5c</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Show me your favorite “Your Natural Nail But Better” shades.</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m64f5c/show_me_your_favorite_your_natural_nail_but/</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1m63ywh</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Looking for a mother of pearl coloured nail polish called “Mermaid”</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>/r/Nailpolish/comments/1m5j6gl/looking_for_a_mother_of_pearl_coloured_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1m639d9</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Are there any clear ridge fillers out there? Colored ones visibly settle into the ridges</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m639d9/are_there_any_clear_ridge_fillers_out_there/</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1m62ym0</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Holo Taco Unicorn No. 1 vs. Sassy Sauce Cock a Doodle Doom vs. an OG UP Polish</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m62ym0</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1m62v1f</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Adding accent nails the next day for a reason to paint and play with magnets 🧲</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m62v1f</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1m62p19</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Shark week!</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m62p19</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1m62o71</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Forever on a mission to dupe Mooncat's Maelstrom in gel 🌊</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m62o71/forever_on_a_mission_to_dupe_mooncats_maelstrom/</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1m62esr</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Opi rapid dry top coat dried half matte</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s0peksfe7cef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1m61tvj</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>Do I need to wipe the inhibition layer between coats?</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m61tvj/do_i_need_to_wipe_the_inhibition_layer_between/</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1m61s85</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Enjoying this underwater vibe.</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jc6gv5s22cef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1m61rdz</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Super Nails</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m61rdz</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1m61alb</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>How similar are ILNP flower child and mooncat midsummer's dream</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m61alb/how_similar_are_ilnp_flower_child_and_mooncat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1m6127t</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>Another Feo, Fuerte, y Formal Post</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6127t</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1m60cuj</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Polar opposite of my normal style. First time ever doing a nude base or a french!</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6tbhve6vpbef1</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1m5zwk3</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>Yoshi 🎮🦖</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5zwk3</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1m5z94g</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Just thought I’d show off my ILNP deep space topped with Mooncat Foxfire</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/l7297wzngbef1</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1m5yuot</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>…and fire featuring the spinny magnet method</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/njyaf6xhdbef1</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1m5xq5y</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Dam Nail Polish Rooster</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5xq5y</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1m5xjlf</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Zoya Haul - if it's still called that in this case</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rlitpjif3bef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1m5xix1</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>High school reunion nails</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7qkeb1aa3bef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1m5xfhm</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>pixel dust is really that girl</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5xfhm</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1m5wuyu</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>If someone wants to start a business selling a magnet spinner I’d happily be your first customer 😆</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m5wuyu/if_someone_wants_to_start_a_business_selling_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1m5w0jx</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Beaded technique after 24 hours of diffusion</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wkxxpqs6saef1</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1m5vxg0</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>Lazy Susan Magnet Setup</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3272byjoraef1</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1m5vtyq</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Gameshow: Spin That Magnet!</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/y3u60550raef1</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1m5vjku</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Help!!</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ygohd0wyoaef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1m5vg2y</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Base question about Monarch Lacquers</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m5vg2y/base_question_about_monarch_lacquers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1m5v41j</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Does anyone know when these are from?</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e8g6zb8zlaef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1m5v05s</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>Am I taking crazy pills or are these two pics of Millennia really deceiving? Like are they trying to make Millennia look bad so we'll buy the new shade? 🤔</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5v05s</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1m5upqd</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>My first Atomic Polish order!</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5upqd</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1m5tubl</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Happy Summerween, babes! 🎃</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5tsv6</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1m5tmi1</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Gel polish peeling? Help! (List of products and steps)</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m5tmi1/gel_polish_peeling_help_list_of_products_and_steps/</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1m5t873</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Recs for brands that have linear holo red, purple/violet, blue and green</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m5t873/recs_for_brands_that_have_linear_holo_red/</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1m5qrsz</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>My first BKL 🐸🦠🦚🧪</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5qrsz</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1m5sml7</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>New fave summer combo! 🌞 💅🏻</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h855jf285aef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1m5sl1i</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>I just want to show off my nail art</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5sl1i</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1m5sb2x</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Mooncat Pandemonium but in other hues?</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m5sb2x/mooncat_pandemonium_but_in_other_hues/</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1m5rk7y</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>For anyone that has used/owned "melt your popsicle" by Orly. I have a question</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m5rk7y/for_anyone_that_has_usedowned_melt_your_popsicle/</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1m5rhdk</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>Your opinion on the *refillable* Bliss Kiss oil pens</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xysklsylx9ef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1m5rhag</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>Update: Cock-a-doodle-doom really is all about the lighting</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5rhag</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1m5rfri</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Recent shimmer manis✨</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5rfri</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1m5rbzf</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>Drugstore Swatches</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5rbzf</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1m5rbp5</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Fun Painted Polish</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5rbp5</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1m5r0m1</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>Recent jelly manis</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5r0m1</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1m5qyfq</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>beautiful summer beige.</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5qyfq</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1m5qrf7</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>Dupe for Icon on Board?</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/onmoteyss9ef1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1m5qftj</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>Drugstore Pink Base</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5qftj</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1m5qf6w</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>Mellow Yellow🌻🌼</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5qf6w</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1m5pxdu</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>ISO the oatmealiest flakie</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ts1bahsan9ef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1m5nwhm</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>💅 Nail polish fans! Help shape the future of custom color &amp; get a gift 🎁</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m5nwhm/nail_polish_fans_help_shape_the_future_of_custom/</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1m5pmhv</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>By the light of the moon</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/s3fq4bfsk9ef1</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1m5plkz</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>Specialty finish Drugstore polishes</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m5plkz/specialty_finish_drugstore_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1m5peec</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>yellow corners of nails only on one hand :(</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5peec</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1m5p0lh</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Amazing blue/green shimmer</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5p0lh</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1m5oqll</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>Is there a polish out there similar to this combo that I did?!</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5oqll</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1m5onhc</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>This one goes to 11… 1130</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5onhc</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1m5ol92</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>Poems for a Harvest Moon on this proud brown girlie</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ekthjile9ef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1m58n7d</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>Long Shot ABeauty Silver Tinsel Topper Polish Search</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m58n7d/long_shot_abeauty_silver_tinsel_topper_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1m5glx1</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Flashing Pink</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vjgk9cxis7ef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1m5jrho</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>why are my nails breaking at the corners</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m5jrho/why_are_my_nails_breaking_at_the_corners/</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1m5o2yp</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>Here to hype Swamp Gloss!!!</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5o2yp</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1m5nrih</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>Cirque Colors will not stop sending spam</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m5nrih/cirque_colors_will_not_stop_sending_spam/</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1m5n7j7</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>So heartbroken about the Mooncat price hikes</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m5n7j7/so_heartbroken_about_the_mooncat_price_hikes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1m5lffx</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>How in the heck do you use a  neodymium bar magnet for glass bead effect?</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m5lffx/how_in_the_heck_do_you_use_a_neodymium_bar_magnet/</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1m5kacz</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>BKL toil and trouble</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/df3kwh3hl8ef1</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1m5k6hn</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>River Styx</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5k6hn</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1m5k1z2</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>My Neighbor Totoro Nails</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5k1z2</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1m5jqmf</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>Where started---&gt; How it's going</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5jqmf</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1m5ji3u</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>🦋🧡Monarch Fluid Art🖤🦋</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5ji3u</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1m5ik8h</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>✨ Touch The Stars ✨</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5ik8h</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1m5i9zx</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>Cracked - Pond Stew / Petals on the Surface</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/x22zowuu68ef1</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1m5i090</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>What is the glossiest and longest-lasting top coat you know?</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m5i090/what_is_the_glossiest_and_longestlasting_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1m5hcdx</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>Bees Knees Lacquer Lovers to Enemies</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5hcdx</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1m5evcj</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m5evcj/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1m5ec6h</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>Uncured builder gel?</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sp0gqclz47ef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1m5dwke</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>Nailbed progress over the past few years</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5dwke</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1m681qq</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>Elegant Swan press ons I made using nail foil</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6bimelxmsdef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1m67a1o</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>Bees</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m67a1o</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1m66dnk</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>Idk about the middle nail... Give me some advice to make the set more cohesive.</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m66dnk</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1m65892</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>finished these fun summer sets today!!</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m65892</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1m64rne</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>bee and flowers</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m64rne</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1m63yni</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>One of my fave sets I’ve done in a long time!!</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m63yni</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1m63a0k</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>Fresh nails, fresh attitude 😌</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yzovlaq0fcef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1m61brt</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>Guava drops 🥝 🍉</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0b4gch12ybef1</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1m60cao</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Polar opposite of my normal style. First time ever doing a nude base or a french!</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ondql76qpbef1</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1m5x0th</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>first time making press ons</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5x0th</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1m5w4m6</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>Tried my hand at cute art!</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5w4m6</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1m5w3lt</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>butterfly wing press ons</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5w3lt</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1m5vv07</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>Give me ideas!!!</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5vv07</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1m5tx27</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Chrome powder - beige undertone?</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1m5tx27/chrome_powder_beige_undertone/</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1m5t7z5</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>Today's work</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a85f0wx99aef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1m5qrpr</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>Hand painted Barbie nails 💕</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5uyyaizus9ef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1m5ng81</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>When I need a little reminder...</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5ng81</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1m5mxao</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>Can I achieve this look without gel polish or an e-file?</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5mxao</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1m5ls11</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>Tuxedo Sam set 🤍</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h1dmlheyv8ef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1m5l37q</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>Any tips on how to make them more realistic?</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zny733xar8ef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1m5jn8y</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>Beginner work</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5jn8y</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1m5j1e8</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>Elemental</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2zn2mytnc8ef1</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1m5gogk</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Weekend Nails</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3ej3if06t7ef1</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1m5ge3b</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>My fourth app, I'm still practicing, what do you think? 🥹</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m5ge3b</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1m5fo5t</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>Something different for my friend. Thoughts?</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/leiwppe9j7ef1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Jul 23 08:13:51 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_07_27.xlsx
+++ b/data/collected_data/2025_07_27.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C510"/>
+  <dimension ref="A1:C734"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9103,6 +9103,3814 @@
         </is>
       </c>
     </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1m737q4</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>my application to be your favourite elf brace face</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/35yl5z7mxkef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1m734uo</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>Am I being picky / paranoid?</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m734uo</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1m72odu</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>Tips</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m72odu/tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1m71vd4</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>Had to get my nails in honor of The Prince of Darkness</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m71vd4</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1m71dwv</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>my chrome spider nails 🕷️🖤</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vi4h47fzckef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1m70pre</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>Did my moms nails</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m70pre</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1m6znyd</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>First attempt at flowers 😍🌸</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6znyd</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1m6z4fl</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>3D Bug Nails</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6z4fl</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1m6yykc</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>Tried nail art for first time</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qhco30rrojef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1m6yj6s</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>First time with long(er) nails in basically forever and love it</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6slf7s3wkjef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1m6y5js</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>help. me.</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6y5js</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1m6w08r</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>Gel x lifting on the tip of my pinky. Stuck everywhere else though</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mpf8kle3zief1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1m6yblj</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>Chrome recommendations?</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hmel6ynzijef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1m6y3p1</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Is this nail plate separation?</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6y3p1</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1m6y1a1</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>new nailsss</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f1s2sxfhgjef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1m6xtl6</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>UV nail polish + base coat/top + cure it ?</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m6xtl6/uv_nail_polish_base_coattop_cure_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1m6xrdc</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>My most favourite nails so far</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6xrdc</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1m6xn4v</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>Does this color look good on me? Any suggestions on other colors I should try out?</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6xn4v</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1m6xc5s</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>Builder gel separating on nail</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m6xc5s/builder_gel_separating_on_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1m6wrl1</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>Controversial Opinion: Soak Off vs. Pull Off</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m6wrl1/controversial_opinion_soak_off_vs_pull_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1m6wpwu</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>Cat eye and flowers</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/os0crr045jef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1m6wlwl</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Got sea shell nails to match the ones I found on the beach 🐚🌊🧜‍♀️</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6wlwl</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1m6w578</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>OPI dupe for DND color</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m6w578/opi_dupe_for_dnd_color/</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1m6w0sl</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>Work at home</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/evl8zov7zief1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1m6vrkz</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>Painting a Hunchback of Notre Dame nail set! Starting with Frollo 😆🙌🏼</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zzp58qu1xief1</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1m6v1xv</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>I need a nail shortened</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rnmte6g5rief1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1m6va6g</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>I think I made a mistake 💀</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m6va6g/i_think_i_made_a_mistake/</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1m6v1v2</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>What do you think?</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t5smbmu5rief1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1m6ukk6</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>Why is this happening?</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6ukk6</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1m6uhbg</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>Why does this always happen</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6uhbg</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1m6u15w</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>for those who saw my last post these are the updated nails tysm for the support!</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/slz8ek6xiief1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1m6u0sx</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>What to do when I don’t want nails for a long time?</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m6u0sx/what_to_do_when_i_dont_want_nails_for_a_long_time/</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1m6tvx1</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>new set</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6tvx1</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1m6tyjw</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>Simple summer floral 🌻</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6tyjw</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1m6tubl</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>my most perfect manicure !</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/csikwdeahief1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1m6t1tr</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>Press ons over Beau's lines help!</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m6t1tr/press_ons_over_beaus_lines_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1m6rtxo</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Which "healthier" method should I use to have nice nails?</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m6rtxo/which_healthier_method_should_i_use_to_have_nice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1m6sgxa</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>My Saracen Order and Experience</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6sgxa</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1m6tmam</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Uñas mal pintadas por debajo?</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/osavjn8ofief1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1m6tktn</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>Glamnetic Lilac Steel</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6tktn</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1m6tjd5</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>Do these look bleh?</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bx91w7z1fief1</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1m6t2qr</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Zoya - Pippa</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6t2qr</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1m6sf4r</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>It's cherry season</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6sf4r</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1m6s6o8</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>I love simplicity</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m4n593ts4ief1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1m6rscz</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>Theme for my engagement party was Berry in Love 🍓</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jdtrrh3v1ief1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1m6rrml</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>These took me WAY too long, but I was so happy with the result!</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o1cur95q1ief1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1m6rq7q</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>One of my favourite designs so far that I've done for a cyberpunk themed shoot</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0mwtsdqf1ief1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1m6rf48</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>Wanted to share my adventure time nails</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6rf48</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1m6qs3l</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>Is there a rings of fire?</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6qs3l</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1m6qmpb</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>Cured Nail strip</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m6qmpb/cured_nail_strip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1m6qmoz</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>My nail artist pulls through for me every time</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6qmoz</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1m6qjd5</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>builder gel suggestions!</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6qjd5</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1m6ptqs</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>Question about how to care for a funky nail</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6ptqs</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1m6qbs7</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>My 8.5 year ills just loves her nails i did for her! Can we show her some love ❤️</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6qbs7</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1m6qax6</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>First time getting almond shape!</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5md0m4v9rhef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1m6q5jz</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>My first Russian manicure</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6q5jz</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1m6pyoo</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Love my new nail tech - UK prices</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6pyoo</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1m6pwu8</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>Matcha green cat eye manicure 🍵🌱</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8qfj16djohef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1m6pwll</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>Adhesive tabs and glue together?</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m6pwll/adhesive_tabs_and_glue_together/</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1m6pt1s</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>are these actually cute?</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vr8bh3gsnhef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1m6otnk</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>Recommendations for at-home gel?</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m6otnk/recommendations_for_athome_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1m6pj84</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>Fairytale Nails..</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6pj84</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1m6pj3t</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Hibiscus 🌺</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/20n0eefvlhef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1m6pinc</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>My nail tech always delivers!!!</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xe4g6jpslhef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1m6oz8k</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>builder gel AND hard gel lifting at the free edge! HELP</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6oz8k</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1m6ot05</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Rainbow nail set</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/626igdtwghef1</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1m6opsk</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>How to break up with your nail tech?</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m6opsk/how_to_break_up_with_your_nail_tech/</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1m6nobe</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>help!!!</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6nobe</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1m6o6nh</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Ombré with magnetic gel</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pwt7qxzrchef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1m6nlgu</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Simple summer mani🌟</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uc3yxmut8hef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1m6ne1b</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>Duck Art Inspo 🪿</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6ne1b</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1m6nbrx</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>I’m naked! 😭 this is your reminder to oil your nails</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/usmsvg907hef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1m6n7v2</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>Fourth Wing Nails🐉</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6n7v2</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1m6n17p</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>Is this normal or do I need a new place</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m6n17p/is_this_normal_or_do_i_need_a_new_place/</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1m6mre7</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>Rainbow Nails I did on myself</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6mre7</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1m6mdyv</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>throwback to Halloween 🫶🏻</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z3pusftt0hef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1m6m2d9</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>Which ones for this weekend? I think the round ones look the best on me but I could reshape any of these technically…</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6m2d9</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1m6l83s</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Nail lamp safety?</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m6l83s/nail_lamp_safety/</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1m6lh6h</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>I just did my nails and I lowkey hate them 😭</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/11i2ml8vugef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1m6kwhb</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>First time in years no color</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z6n6ujf3rgef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1m6kv38</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Why are these flat white lines on my daughter’s nails? They’re becoming more pronounced as the weeks so by.</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6kv38</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1m6kmdv</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>Nail glue strong enough for bartenders?!</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m6kmdv/nail_glue_strong_enough_for_bartenders/</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1m6k7w3</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>Clionadh - Baeocystin</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6k7w3</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1m6dt2o</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Builder or poly?</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m6dt2o/builder_or_poly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1m6jp4k</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Adhesive Nails</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m6jp4k/adhesive_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1m6jmpa</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>iridescent candy gloss 💿🍬🫧</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6jmpa</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1m6imnq</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>A nightmare somewhat fixed, please don't say you can do a set if you cant</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6imnq</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1m6j4wo</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>“kiss classy nails press on pack”</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5b9tlbfgfgef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1m6ijfm</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>what do we think of this color?</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6ijfm</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1m6i9x7</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>How bad are these?</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6i9x7</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1m6h7nz</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>Cheated on my favorite nail place… never again</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6h7nz</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1m6hexf</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Nail shape for working nails?</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6hexf</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1m6h605</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Midnight Sky</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6h605</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1m6h27j</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>silly little set</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6h27j</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1m6946c</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>Should I get a new lamp for gel nails?</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m6946c/should_i_get_a_new_lamp_for_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1m6gwu0</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Nail rebuild</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m6gwu0/nail_rebuild/</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1m6gn8q</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>Gel polish is not for me but this mani is cute</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6gn8q</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1m6gg46</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>5 days in</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6gg46</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1m6gfy0</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>Cat eye is my fave base. Tell me yours.</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6bp83xfdxfef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1m6gaxy</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Press ons from Amazon!</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6gaxy</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1m72uhr</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Sand Viper</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/el30ylbftkef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1m71jpl</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Silver chrome ✨</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/984ckqpqekef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1m710ub</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Request: Cirque Cupids Arrow and Mooncat La Petite Mort</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m710ub/request_cirque_cupids_arrow_and_mooncat_la_petite/</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1m70pcv</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Anyone know of any other photothermals besides Death Valley nails?</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m70pcv/anyone_know_of_any_other_photothermals_besides/</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1m70c36</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Finally trying Snow Can Wait</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m70c36</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1m70c1d</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Finally trying Snow Can Wait</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m70c1d</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1m6zssi</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>any idea what this gorgeous purple that mia maples has on in this video is?</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6zssi</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1m6zrtr</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>A veces de Barbie</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/32scalhewjef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1m6zpnj</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Cuz I’m a punk rocker yes I am</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6zpnj</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1m6ytr8</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>When I go bright, it has to ✨shimmer✨</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6ytr8</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1m6y4mj</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>First time magnetic user!</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6y4mj</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1m6xlbm</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>Thoughts on this product / ingredient list? Will it do what it says?</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6xlbm</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1m6xjku</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>most compliments i've ever received on my nails</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p0fa66q0cjef1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1m6x3y5</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>Looking for some neons/brights</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m6x3y5/looking_for_some_neonsbrights/</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1m6wbzx</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>Little sunset 😊</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3p68dasv1jef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1m6vzy8</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>A groovy new mani</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3efpq6k0zief1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1m6ve0n</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>So pink it burns my eyes</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qvxeair0uief1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1m6v6l1</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>Little happy Pond Stew frog</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6v6l1</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1m6uq7p</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Strawberry Milk Nails!</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0sxmr9ofoief1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1m6ug9n</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>Best turning magnet setup??</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m6ug9n/best_turning_magnet_setup/</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1m6ufyq</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Did I buy the absolute WORST thinner possible?</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6ufyq</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1m6uerj</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>Solar nails in the desert sun is are the most fun</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6uerj</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1m6u9la</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>ILNP Daytrip</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6u9la</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1m6u8ca</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Holo Taco Sky Lounge + a matching sheer jelly on top to deepen the color (and the dog tax is paid 🐶)</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6u8ca</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1m6tyqa</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>Psilocybin w turning magnet!</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/w0d7cca9iief1</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1m6tufc</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>The most complimented color I’ve ever worn</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6tufc</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1m6tjnm</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Help!! Can’t get nail polish to last more than 1-2 days</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m6tjnm/help_cant_get_nail_polish_to_last_more_than_12/</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1m6tcbp</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Funfetti!</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6tcbp</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1m6ta4w</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>ocean nails🌊🏖️</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6ta4w</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1m6t7oz</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>Hypnotic</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6t7oz</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1m6t38i</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Is anyone disappointed in Orly 90s box?</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m6t38i/is_anyone_disappointed_in_orly_90s_box/</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1m6su1q</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>New favourite magnetic! 🧲</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6su1q</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1m6scv4</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>Got proposed to while wearing Ether Moon 🧚🌘✨</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6scv4</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1m6r6w0</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>Best top coat for magnetics?</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6r6w0</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1m6r3pf</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>Need help choosing summer nails</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m6r3pf/need_help_choosing_summer_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1m6qlat</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>neon green summer skittle! 💚</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6qlat</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1m6qid3</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>Not over 2010s galaxy nails</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ykjnr5sarhef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1m6qhmv</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>Best nail file for short natural nails that are prone toward breaking? I'm trying to file them gently and hopefully grow them out.</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m6qhmv/best_nail_file_for_short_natural_nails_that_are/</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1m6qb6k</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Been in a blue kind of state of mind this summer</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eond2u0crhef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1m6q07l</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>UberChic opinions?</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6q07l</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1m6puen</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>One of my favorites so far!</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6puen</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1m6pu4o</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Help! Tell me your tips and tricks for nail filing</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m6pu4o/help_tell_me_your_tips_and_tricks_for_nail_filing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1m6pspr</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>Flayer of Minds</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6pspr</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1m6pdcb</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>My favorite so far!</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xpureojrkhef1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1m6paxc</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>✨BKL’s Bog Dweller✨</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/10rpyddnghef1</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1m6ozmn</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>La Llorona by Uno Mas Colors</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pi9lo9h5ihef1</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1m6oplp</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>How do we feel about this for nails?</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tn9qhkiaghef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1m6onle</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>ELI5: Magnetic Polish Techniques</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m6onle/eli5_magnetic_polish_techniques/</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1m6olgy</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>Super sick rn and my nails are the only thing healing me 🐞</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6olgy</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1m6o9og</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>✨Fancy Fingers✨Christian Louboutin</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w2usq3vbdhef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1m6nqvw</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>Mmmm car nails are the best 💅🏻</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5bh6ongs9hef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1m6nq9i</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>Current mani🌱</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6jtdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1m6nm6k</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>Polish protection</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kt980dpj8hef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1m6nhfr</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Superman inspired nails!</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/imnqm2h28hef1</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1m6n6tw</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>I've just ordered my 1st fancy polishes! Magnet advice please experts</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a5kvl0u36hef1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1m6meqg</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Rainbow silver holo 🩶🌈</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6meqg</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1m6m2p2</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>Help me decide what to do!</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6m2p2</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1m6ly33</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>Dupe for Essie Play Date? Ideally a gel option...hit me!</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m6ly33/dupe_for_essie_play_date_ideally_a_gel_optionhit/</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1m6lh4m</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>I’ve got the sky on my nails ⛅️</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6lh4m</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1m6ktt6</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>My small growing collection 🥰</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6ktt6</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1m6kni1</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>Magellanic Clouds by Masura</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vy49o7yepgef1</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1m6kmbp</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>Does this nail shape do me any justice?</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6kmbp</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1m6kefs</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>Linear Polish vs. Linear Topper</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m6kefs/linear_polish_vs_linear_topper/</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1m6k8zn</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>Clionadh - Baeocystin</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6k8zn</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1m6k8au</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>Im looking for a light pink-subtle glimmer nail Polish like the below but everything I try has too chunky pieces of glitter or the glitter doesn’t have that super light iridescent quality. Are there any good products that can help me get this that aren’t gel?</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nlgtwsgmmgef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1m6hvcs</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>DIY Helmer inserts</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m6hvcs/diy_helmer_inserts/</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1m6jytz</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>Any recommendations for a one-coat and/or quick dry Tiffany blue, please? Creme or shimmer doesn’t matter</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m6jytz/any_recommendations_for_a_onecoat_andor_quick_dry/</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1m6jxqt</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>A little in love with matte 😍</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/btuyy0ypkgef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1m6jwrh</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Holo Taco Unicorn No1</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6jwrh</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1m6hxzj</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>This immediately became a contender for my favourite polish ever, I can't cope with how shifty and sparkly it is!</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/z2d2xbtg7gef1</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1m6hgx5</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>Affordable (and cruelty free) Cremes?</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m6hgx5/affordable_and_cruelty_free_cremes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1m6hep1</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>Day by Day by Night</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6hep1</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1m6hdkv</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>That one problem child nail</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6hdkv</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1m6hdks</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>Got complemented on my nails today and I've been giggling nonstop</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d6dexqqn3gef1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1m6gyg8</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>One of the polishes that I made at the Polish and Beauty Expo</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bmsdq0us0gef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1m6gint</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>I love cremes so much.</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3uoemilvxfef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1m6g9a3</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Can you stamp with solid gel?</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m6g9a3/can_you_stamp_with_solid_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1m6g7hk</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>Do you "plan" your next manicure...</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m6g7hk/do_you_plan_your_next_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1m6fr2z</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>Sassy Sauce Polish for the last few weeks</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6fr2z</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1m6fqy3</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>Am I tweaking or is this absolutely not my color?</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6fqy3</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1m6fk9r</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>How long is too long 🤔</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6fk9r</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1m6fgty</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>Color combo 💕</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6fgty</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1m6fd2m</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>Ok I Get It Now -Lurid Lacquer Shimmers Are Amazing!</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6fd2m</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1m6f7ac</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>I rarely where just one color but…</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6f7ac</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1m6f0uy</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>Favorite ultra fine particle shimmers?</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/thv3p36hnfef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1m6f01z</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>So impressed with this combo!</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/loxqltmbnfef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1m6ewvb</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>UF Glow👽💚</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6ewvb</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1m6evxg</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>Easiest home system for basic manicure</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m6evxg/easiest_home_system_for_basic_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1m6e1xz</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>Pink red clash</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6e1xz</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1m6e04w</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>Summer on my nails</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6e04w</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1m6dr78</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>Looking for this Gel Polish - #34 sheer nude with blue shimmer.</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6dr78</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1m6dk9q</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>Recs?</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m6dk9q/recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1m6cxbe</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>First polished for days order called for a glowy skittle</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/37j5qpzd7fef1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1m6abfz</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>maylandia by prism polish</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z3o83lblieef1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1m72yw5</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>3D Sculpting Gel Not Sticking?</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1m72yw5/3d_sculpting_gel_not_sticking/</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1m6ou4m</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>Before I let these go</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p6c4cqa5hhef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1m712nj</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>Rainbow Sailor Moon 🌈🌸✨</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fatuxlnm9kef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1m6xme9</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>Baby shower nails. Orange Cutie themed 🥰</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kq3asbmtcjef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1m6xa13</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>My neighbor Totoro set</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mmp8l5ys9jef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1m6x7hf</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>It's colorful😍</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w8u9kxe49jef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1m6wxgn</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>nails with bows ☺️</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qd68xkxu6jef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1m6vpfm</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>Painting a Hunchback of Notre Dame nail set! Starting with Frollo 😆🙌🏼</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/g8gv6ytkwief1</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1m6vba2</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Saw this on Pinterest...</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bp480qhdtief1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1m6smxg</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Butterfly/ fairy nails</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/acwzo7678ief1</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1m6s9en</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Product help!</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1m6s9en/product_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1m6ril4</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>Seattle ideas?</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6ril4</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1m6rczu</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>My Chemical Romance - The Black Parade themed press-ons🤘🏻</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h1x8rnrsyhef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1m6lqi2</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>Set for my mom (beginner)</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6lqi2</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1m6kflb</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>What do you think of these nails that I made for marriage proposal?</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ho11djyngef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1m6k8sw</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>Estas son las de hoy 💅</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aruvk4plmgef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1m6jd73</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Evil eye 🧿 art on natural nails 💅</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6jd73</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1m6j89q</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>My favorite nail set I’ve done so far.</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ak4duo03ggef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1m6inst</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Today's work</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0hiakwh8cgef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1m6h0uj</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>🐰simple LADS themed set 🐈‍⬛</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6h0uj</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1m6gybc</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>Butterfly nails done by me 🦋</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7xpa8hsr0gef1</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1m6flrn</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>my art</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6flrn</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1m6fkdn</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>my favorite place</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6fkdn</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1m6eftr</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>Fourth Wing Inspired Nails 🐉</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6eftr</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1m6ea5u</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>Anyone have any ideas on what to do for these last two nails?</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rvnb44ezhfef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1m6cfkn</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>Lemon Drop nails (beginner)</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i3moae783fef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1m6bt4v</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>Summer pink ice cream</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yflewm7lxeef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1m6a61q</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Pokemon porcelain set</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6a61q</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1m4sv93</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>Cat eye</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m4sv93</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1m4j1nv</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Today's challenge is a cowboy style nail</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m4j1nv</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Jul 24 08:13:53 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_07_27.xlsx
+++ b/data/collected_data/2025_07_27.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C734"/>
+  <dimension ref="A1:C926"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12911,6 +12911,3270 @@
         </is>
       </c>
     </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1m7ympb</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>How to shape my nails</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ijep0iz76sef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1m7x5eq</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>First time doing gel nails with forms</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m7x5eq/first_time_doing_gel_nails_with_forms/</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1m7x3pj</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>indents from electric nail file</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/695l7qf8pref1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1m7wza8</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Late night experiments</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m7wza8/late_night_experiments/</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1m7wk98</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>How to strengthen my nails</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7wk98</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1m7wdby</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Got these done a week ago!</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l3q2kkgehref1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1m7w8ny</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>Red vives 🍒 🐞</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h0e29p82gref1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1m7sejj</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Gel Polish Advice? (beginner teen tech!)</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m7sejj/gel_polish_advice_beginner_teen_tech/</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1m7vzxp</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>They remind me of a colorful villain</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7vzxp</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1m7vpgq</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>How to strengthen natural nails</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p1mvlmyiaref1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1m7tf6z</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>Should I get this fixed?</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nqwhhptloqef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1m7ue50</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Gel , Shellac, Acrylic ? Help!!</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m7ue50/gel_shellac_acrylic_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1m7v45b</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>My nail is red / bruised. Idk if it’s from drilling too far or what? I started using gel , but it has never bothered me or anything.</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ql6izmkj4ref1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1m7uzmm</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>nails i got done yesterday</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cjn96i173ref1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1m7ufym</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>Did my own nails for the first time</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/edxbihc1yqef1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1m7ua4d</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Birthday SpongeBob Nails</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7ua4d</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1m7tnf4</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>First time with painted nails, getting OCD about scuffs and scratches.</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7tnf4</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1m7tkm3</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>I wanted them to be more yellow</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g2yvvs6zpqef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1m7t79q</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Soft Candy Colours with a Twist</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7t79q</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1m7t71s</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>I cant stop staring at my nails 🥹✨</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8zl878qlmqef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1m7t4vw</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>Did my first blooming … what you guys think? I messed up one nail I tried to do a flower</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2rg424a3mqef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1m7sqkx</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>Liquid latex - two ways</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7sqkx</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1m7smom</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Went out of my comfort zone… bright red with some gold!</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7smom</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1m7sg8r</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>2022/23/24/25 birthday nails. Bestttt?</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7sg8r</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1m7sevn</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Omg I’m so in love with this set! 😍😍</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7sevn</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1m7se9q</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>skz dominate tour press-ons</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/863z9rvffqef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1m7sb4k</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>Warped tour nails!</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lfdt5czoeqef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1m7roib</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Great top coat?</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m7roib/great_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1m7rb12</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>First time using nail tips - advice?</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7rb12</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1m7qux2</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>My techno fest nails by @siczmo</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/841ep8ne2qef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1m7qof2</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Can we talk about my nail glow up lol</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7qof2</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1m7qeqq</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>Extend the life of your nail polish?</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m7qeqq/extend_the_life_of_your_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1m7qa4w</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>Decided to get back into it. Here are some of my random nails!</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ybfs3fthxpef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1m7puz4</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>Cat eye ombré with pink nails</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p8jx4wlwtpef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1m7putz</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>Dried flowers 🌸🪻</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/arrz41gvtpef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1m7pcrg</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>“mermaid” set i did on my friend</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7pcrg</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1m7pboc</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>Cousins’ nails with Lisa frank stickies! Rainbow cat eye top coat for a retro holo sticker effect!</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7pboc</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1m7p728</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>Next style! Still practicing, but think I'm getting better</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pgvenw4iopef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1m7p51k</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Summer blue vibes 😻</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7p51k</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1m7nmrr</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>How do I know which polish is base gel and which is the soak-off gel?</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7nmrr</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1m7nzs6</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Concert nail ideas?</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s9hlyxv0fpef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1m7obqi</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>How do you fix a chipped nail like this?</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d463kjykhpef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1m7o8fl</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Nobody trims the cuticle anymore !</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jc86dvbvgpef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1m7mca3</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>tried out tortie accents for my 3rd attempt at structured gel! sharing my first 3 sets</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7mca3</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1m7osn8</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Y’all liked my nails so much last time, here’s my boyfriend’s Warhammer nails</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q8v6h6i9lpef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1m7ouxj</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>New gems after 4 weeks</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7ouxj</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1m7oqqm</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>Update on my Sad Nails</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7oqqm</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1m7o06l</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>Protecting nails after unfortunate gel removal?</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m7o06l/protecting_nails_after_unfortunate_gel_removal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1m7nvt3</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>Cat Eye on Bare Nails. 🤍🖤</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7nvt3</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1m7ntkz</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>Any recommendations for a gel base similar to this?</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7ntkz</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1m7nqr6</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>Builder gel over press ons...</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7nqr6</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1m7nnpo</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>I usually make them myself but this time I paid to have them made for me☺️</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7nnpo</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1m7nn4a</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>Zoya - Marley</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7nn4a</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1m7ndxr</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>First time getting them done, went with something low-key, was not disappointed 😁</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7ndxr</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1m7n6vs</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>Press ons but I loved them!!</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7n6vs</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1m7mloe</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>Mommy daughter matching shorties. They’re a little big for her nails but still cute</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/db5dbp2t4pef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1m7m45h</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>Loving myself a matte leopard</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0nuppdnc1pef1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1m7lptg</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>My favorite set so far! I started making press-ons three days ago, so any tips are welcome.</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g8ltfoijyoef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1m7lmq6</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>short nails to play the guitar 💅🏾🍒❤️</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ajc4s7yxoef1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1m7lii9</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>Can’t seem to find a clear cat eye gel with green shimmer!!</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7lii9</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1m7l9ww</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Fiji Wave Inspired Nails 🌊</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7l9ww</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1m7lcz7</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>my friends chose the design for these 🍓</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7lcz7</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1m7lacm</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>Summer Mermaid Vibes</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/adfoa66kvoef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1m7ktxr</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>Why is the ring finger nail bending inward?</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7ktxr</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1m7kzbp</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>Could I get these painted over instead of a refill?</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7g3qabmgtoef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1m7l168</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>first manicure in a couple years!</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wio2jndutoef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1m7kmam</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>First set in 2 years</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7kmam</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1m7k7l5</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>Review nails steamer</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/zr2ep4/does_steam_work_for_removal_says_it_works_on_gel/?share_id=hJ0o__rrb_u28Mq0zYzuY&amp;utm_content=2&amp;utm_medium=ios_app&amp;utm_name=ioscss&amp;utm_source=share&amp;utm_term=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1m7k4se</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Teacher nails?</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7k4se</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1m7j9jt</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>BIAB/Gel/Builder gel recommendations</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m7j9jt/biabgelbuilder_gel_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1m7iz00</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>Fish Nails!!!</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wltmsksrfoef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1m7izqc</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>80’s inspired summer nails on polygel</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7izqc</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1m7ixae</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>My cousin made them for me</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xhht7begfoef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1m7ivx7</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>Cowboy Carter press on nails!</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7ivx7</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1m7ivcp</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>Just got my first ever set with my bestie for a vacation and I’m in love</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7ivcp</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1m7itcq</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>10 day grow out normal?</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7itcq</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1m7io99</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>in love with the result I got</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2bz0y8yrdoef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1m7in3x</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>A bit of an extra set for an event 💗</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7in3x</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1m7i2qh</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Short and (sugar plum) sweet...and the difference with a good tech!</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7i2qh</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1m7hzwc</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Fresh</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g59uhc969oef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1m7hwbi</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>These are the nails of a killer ✨</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7hwbi</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1m7g7db</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>How do you like this funny manicure just made</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tj7fuih6xnef1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1m7gx3s</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>onycholysis help</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m7gx3s/onycholysis_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1m7gd2r</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>Does anyone know what this is?</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7gd2r</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1m7g89l</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>22nd birthday nails!!</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7g89l</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1m7gldz</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>FINALLY went to a private nail tech! The vibe is ✨deep blue sea/siren✨</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7gldz</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1m7gddj</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Beach Nails</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7gddj</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1m7fgq5</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>My nail artist killed it! Sleep Token inspired.</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7fgq5</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1m7fp99</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>Purple chrome</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7fp99</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1m7fnuj</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Nothing fancy but I love it🍎🍏🫶</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7fnuj</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1m7ff32</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>First time trying French myself on my natural nails</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wbioq2cxrnef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1m7fbah</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>Attempted with non UV "gel" for the first time</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d62oait7rnef1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1m7fa0k</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>another tb</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n5v0rfuyqnef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1m7f9yf</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>🍒🍒</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7f9yf</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1m7ezmu</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>Which nail polish would you choose?</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7ezmu</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1m7f58l</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>Some recent nails (done w nail stickers)</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7f58l</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1m7epi3</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Mario Kart inspired nails</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7epi3</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1m6xtpx</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>Help!! I can’t take the rest of the gel x nails off</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m6xtpx</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1m7ekih</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>AHHH MY BIRTHDAY BEACH NAILS LOOK SOOOOO GOOD</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7ekih</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1m705lb</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>allergic reaction?</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m705lb/allergic_reaction/</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1m7xarg</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>Ruined cat eye nails</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qd44eewbrref1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1m7vwp5</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>Swatch request: KBshimmer + Phoenix toppers (and one DVN)</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m7vwp5/swatch_request_kbshimmer_phoenix_toppers_and_one/</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1m7vtrc</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>same polish, different nails</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7vtrc</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1m7ufe4</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>Magnetic nail polish virgin</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k8cs4o8wxqef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1m7uc6n</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>Newbie here</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nhe77mp3xqef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1m7u79g</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>bkl he is coming🌑🥀🏰</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0qp7oohtvqef1</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1m7t50g</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>is nail filler a thing?</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4bn9osm4mqef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1m7stin</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>Liquid latex - two ways</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7sqkx</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1m7rdwq</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>First Shimmer polish!</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7rdwq</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1m7rbu4</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>Do you folks know of more polishes that are dupes to these?</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7rbu4</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1m7qrpx</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>millennia respect/appreciation post</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7qrpx</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1m7qjm2</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>Described as a bright red neon crelly with a strong blue/purple shifting shimmer.</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/13xkn70rzpef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1m7qc8w</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>Green lace frenchies</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7qc8w</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1m7pnge</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>Another electric blue added to the collection</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7pnge</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1m7pj2h</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>Kbshimmer topcoat darkening?</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xv6t2dg7rpef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1m7oo3h</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Holo Taco Unicorn No. 1</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7oo3h</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1m7omkh</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>Current mood</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7omkh</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1m7nx7g</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>Playing with jelly</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7nx7g</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1m7nqxu</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>Dollar tree came through today!!!!</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7nqxu</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1m7nmvj</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>Iridescent summer nails🐬🪷</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rg4nceibcpef1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1m7nd6j</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>Homebrew Dupe</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cns5mus8apef1</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1m7n85q</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>Shopped my collection and rediscovered this gem</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/10hjt8ja9pef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1m7my2u</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>Donut party, y’all 🍩</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i55dpif97pef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1m7mo6x</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Mooncat - Moonfairy (Matte Edition!)</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7mo6x</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1m7mlif</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>tried tortie accents for my 3rd DIY gel mani!</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7mlif</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1m7mfr1</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>Is there a safe way for me to wear press-ons?</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f20f7i7n3pef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1m7mffk</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>Set escultural con rojo coral flúor</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/onidd1uk3pef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1m7m4c7</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Emily de Molly Mystic Forces</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7m4c7</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1m7lpp2</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>Windchime spinners: a safer way to spin a magnet!</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ymq7h5biyoef1</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1m7lh0x</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>First Attempt at an Almond Shape</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b433s5wuwoef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1m7lgtq</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Honest Review of Blank Beauty Polish</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7lgtq</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1m7lcno</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>Thrift haul: Which should I start with ?!😍</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ljqud8s0woef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1m7l5hs</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>Trying to decide on my next mani color</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7l5hs</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1m7k28r</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>Help me make a decision for me first purchase</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1axzeuszmoef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1m7k1g9</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>Preventing Skin Under Nails From Ripping From Nail</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m7k1g9/preventing_skin_under_nails_from_ripping_from_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1m7jlj9</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>Follow up for Orange Recs 🍊</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7jlj9</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1m7j9u8</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Update to falling out of love with doing my nails, it feels nice to see color of any kind on my hands again ♥️</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7j9u8</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1m7i9qm</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>looking for a dupe of this nail polish</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7i9qm</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1m7hga0</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>Is there a way to make white gel glow red in the dark?</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m7hga0/is_there_a_way_to_make_white_gel_glow_red_in_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1m7gw6z</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>taking advantage of prenatals to finally grow my nails out</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7gw6z</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1m7gp1m</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Are we still doing fishing lure nails?</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7gp1m</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1m7esht</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>ILNP midnight kiss in matte?</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m7esht/ilnp_midnight_kiss_in_matte/</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1m7e85u</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>Calling chemistry friends: How do topical nail proteins like NailTiques Formula 2 actually work?</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m7e85u/calling_chemistry_friends_how_do_topical_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1m7dthh</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>You folks were not kidding</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qog0zxrygnef1</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1m7dmxv</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>Clionadh Cosmetics - Planetary Attraction</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/u9pq4p7ufnef1</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1m7dg7x</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>Limelight</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7dg7x</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1m7d1hq</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Nail edge is really far down on finger?</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t020m0lranef1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1m7cvnl</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>Feeling like a mood ring</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7cvnl</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1m7cb7k</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>A sweet pair 🍬</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7cb7k</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1m7c1dl</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>Nailtiques/peeling nails question!</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m7c1dl/nailtiquespeeling_nails_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1m7bqbd</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Quick dry top coat over thicker top coat? Or two coats of QDTC?</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v81cvenk2nef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1m7baed</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>Cirque Ballet Slipper</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8w2o1vs00nef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1m7audz</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>Is there a linear holographic polish that also looks good indoors?</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m7audz/is_there_a_linear_holographic_polish_that_also/</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1m7am8a</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>Loving this Essie polish I randomly picked up</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7am8a</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1m7akpp</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>Bachelorette</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7akpp</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1m7aiys</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>Those who kinda fell out of love with doing your nails, how’d you get back into it?</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m7aiys/those_who_kinda_fell_out_of_love_with_doing_your/</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1m7aatu</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>Similar polishes to Sorbet’s ‘Coconut Ice’</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7aatu</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1m79w2j</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>Polishes similar to swamp sparrow by DVN?</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qe4q9vt7qmef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1m79lqi</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>ORLY “GRLPWR” 🍒</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m79lqi</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1m792nk</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>ooh so buttery 🧈 💅</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m792nk</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1m78z4b</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>Cirque Color Matching</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m78z4b/cirque_color_matching/</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1m78sc3</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>Holo Taco Unicorn No. 1</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m78sc3</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1m78dyu</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>I trusted y'all on LA Colors</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8mbvzosqemef1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1m7843b</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>1 minute mani</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7843b</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1m77u4n</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>🩵💙Blue Sunburst💙🩵</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m77u4n</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1m779xw</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>Got nice motivational manicure. Thought it would be a fun idea 😅👌</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m779xw</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1m779k6</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>I've changed my nails 3 times this week 🙈</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m779k6</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1m75t1c</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>Cirque Colors - Mood Ring (Matte)</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m75t1c</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1m756ot</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>PSA (that I am probably the last to know lol)</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ebotzj7rklef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1m74m8w</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Earth to Gaia</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/irn9v7eeelef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1m7yjhn</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Unintentionally beachy set! 🌊</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ituolq295sef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1m752w5</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>Idea Suggestions For Nail Art</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1m752w5/idea_suggestions_for_nail_art/</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1m7lr18</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>Abstract :D</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9x89c75syoef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1m7w1qh</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>leopard print 💅 nails</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7w1qh</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1m7ukrv</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>Jelly cat nails</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9tuydtq9zqef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1m7twlx</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>Cat eye polish, but make it bear-y artistic. 🐻</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/55exmuy0tqef1</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1m7tvii</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>I like to do my own nails, this is the most recent one</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7tvii</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1m7t57r</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>Kept It Playful, Not Crazy — Just Enough to Get Noticed</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7t57r</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1m7r4g7</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>Gone fishin nail art</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7r4g7</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1m7qbpq</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>Finally able to get back to painting/filming! In my excited here is some of my random nails I'm either okay to pleased with.</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6e41jxovxpef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1m7q9b2</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>custom nails for a friend</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rajhf60bxpef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1m7mp6r</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>Beach nails (removed because of car pic)</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7mp6r</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1m7k9ua</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>Vans warped tour</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7k9ua</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1m7j6qu</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>3D Gel Help</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7j6qu</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1m7i87l</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>do you like it?</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5mlkrluraoef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1m7flqp</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>Today I made this design, do you like the color?</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rwsptfg5tnef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1m7cz6j</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>Feels electric...</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eaxubf0ibnef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1m7cumo</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>these were so fun but took me so long to do 😭</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7cumo</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1m7b8vs</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>bday nails!!!</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7b8vs</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1m7ar9p</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>beautiful nails</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7ar9p</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1m7ajx5</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>Nice colors</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gqc4sr4xumef1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1m7agck</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>🤍🎀🩷</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m7agck</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Jul 25 08:13:39 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_07_27.xlsx
+++ b/data/collected_data/2025_07_27.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C926"/>
+  <dimension ref="A1:C1126"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16175,6 +16175,3406 @@
         </is>
       </c>
     </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1m8ss6e</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>fresh set after a month and a half</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f1m4lgff2zef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1m8srp7</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>Freestyle press on set</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7lv91gm92zef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1m8so7u</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>Natural nails</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xgwpn8c51zef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1m8s8i8</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Cherry Bomb 🍒</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fj88dwjawyef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1m8rlwf</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Will my nails last longer by putting the gel polish directly on my nails, or putting it on press-ons?</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m8rlwf/will_my_nails_last_longer_by_putting_the_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1m8oesl</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>Neapolitan Rilakkuma set inspired by Aislingstudios and Pinterest photos</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8oesl</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1m8pkwc</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>New Nail Tech, How did she do?</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8pkwc</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1m8qbef</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>New manicure.. tell me what you think.</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8qbef</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1m8n6ft</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>Slammed my nail in the door 5 months ago</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s161odctixef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1m8q25q</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>Wanted to go for a galaxy vibe with only drugstore polishes... How'd I do?? :3</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/y9201vra9yef1</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1m8pvyq</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>Practicing smaller details (beginner) — I’m happy with how these turned out!</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g60sf1dn7yef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1m8pr1w</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>My Miami Nails. I used clear tips for length. Kinda made a mess with the glow powder lol</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8pr1w</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1m8plvn</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>My first time making 3D cherries🍒💅🏼</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vu8eqiay4yef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1m8p6d0</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>Looking for true translucent nail chrome powders… has anyone tried any of these, or any others?</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8p6d0</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1m8ok8c</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>Normal for nails to feel tender?</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m8ok8c/normal_for_nails_to_feel_tender/</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1m8ok1b</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>My "summer fairy glen" set 😊</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uvcjucg3vxef1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1m8off7</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Vertical ombré</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dva8mpyytxef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1m8oe6n</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>Tb to my Christmas set 🫶🏻</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ac2n4ektxef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1m8odqp</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>Some nails I did this week!</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8odqp</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1m8nvs9</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>Power of the puss set</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5lefl1s1pxef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1m8nuz7</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>bluebs</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8nuz7</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1m8nqts</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>Pretty 🤭</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qx4mtf3unxef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1m8nm8p</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Could I extend my natural nails to longer coffin shape?</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0j74d47qmxef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1m8n19m</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>Tried xtra short square for the first time</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8n19m</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1m8mba5</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Color vibe - feeling it</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8mba5</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1m8map1</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>What color should I pick?</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8map1</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1m8m681</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>What can you tell me about this work?</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5kyqotu5axef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1m8m1c6</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>Tips to Improve Using Non Dominant Hand?</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m8m1c6/tips_to_improve_using_non_dominant_hand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1m8m0h2</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Which Opi color??</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rhxhppcr8xef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1m8lqkr</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>I asked my nail tech for “pink vibes” and she absolutely killed it 😭🩷</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8lqkr</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1m8iyyn</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>They turned out even better than my inspo pic</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8iyyn</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1m8k05j</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>first manicure</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8k05j</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1m8l0wy</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>How can you get rip of these lines? It is not smooth as other have done their. it</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8l0wy</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1m8k2jl</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>Bold turquoise + cool glitter: a combination that dominates looks</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bzo07akiswef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1m8jq9y</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Cat eye ombré on natural short nails</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8jq9y</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1m8jkhm</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Just trying some shroomies. Leaning towards no background, only mushroom.</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gmfn9giiowef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1m8jj9c</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>Can you let me know if I’m being too picky?</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8jj9c</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1m8jj91</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>Acrylic lifting after a week. Is it always the due to the application technique?</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m8jj91/acrylic_lifting_after_a_week_is_it_always_the_due/</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1m8jcgz</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>I made these 🫒</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8jcgz</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1m8j32h</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>the nail tech is rude but did a great job,should i go back next time?</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xqyfq7bskwef1</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1m8iw1a</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Any idea why my nails on my right hand all have a weird shaped nail bed?  I can’t figure it out!</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ac3rgenbjwef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1m8i0tz</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>Recommendations for a manicure set ?</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m8i0tz/recommendations_for_a_manicure_set/</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1m8hzqa</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>New French Mani</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8fbiycofcwef1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1m8gnlu</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>My first short almonds</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8gnlu</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1m8gms5</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>My mini art gallery</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8gms5</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1m8g7dg</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>More pictures of my press ons</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8g7dg</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1m8g3kp</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Tried something new 💅🏽</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eeqbax5lyvef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1m8fdpc</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>barbie fairytopia inspired nails🧚🏼‍♀️</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8fdpc</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1m8fd93</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>Does anyone have a guess on what this OPI shade is?</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8fd93</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1m8f10b</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>Being your own nail tech is rough🥹 but the outcome is always worth it</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/q21xmz4nqvef1</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1m8eyze</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>romantic 💅</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lxj38x8pqvef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1m8eysw</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>Nail shape</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8eysw</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1m8e95w</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>how long do you think till i can do gel x?</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/54w0v2zrlvef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1m8e5tt</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>Pink nails with a bow, very delicate</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1qyxbcb3lvef1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1m8e47l</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>Would you rock these intricate black nails?</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k6b921irkvef1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1m8dc6z</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>How do I shower?</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p40e3omcfvef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1m8d7ga</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>Abstract nails</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1h1tanvgevef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1m8dx26</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>Lizzie McGuire who??? (done by Jocelyn of course)</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8dx26</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1m8dw15</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Manicure and pedicure today</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8dw15</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1m8djlo</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Some neon vibes 🩷💙</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gp2m0fisgvef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1m8da94</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>More shiny press ons ✨</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/usqt0w30fvef1</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1m8d7zg</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>These look bad right? I asked for them to be rounded but my sister said my thumbs look like clown shoes.</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/i3ZF41k</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1m8cze0</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>Pink Marble w/Glitter</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8cze0</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1m8bqze</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>Chrome nails</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zlq01duk4vef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1m8b2kl</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>Which shape suits me better?</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8b2kl</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1m89g88</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>My polygel has a sparkling layer how do I stop that</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ub0jok8apuef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1m8azci</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Need assistance making my own Press-Ons (I hope this is okay!)</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5014n30hzuef1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1m8akas</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Shaping my nails for finger picking guitar</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8akas</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1m8aibt</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>My attempt at a retro manicure. Any thoughts?</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bh56d2oawuef1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1m8ag8l</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>Had a chance to do a long set. And yes they're too long!! 😅</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/suhev0twvuef1</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1m89wzo</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>Vacation memories of this manicure</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/chjgkk5esuef1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1m89tna</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>Summer nails</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m89tna</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1m89t2u</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Is hard gel the best option for me?</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m89t2u/is_hard_gel_the_best_option_for_me/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1m8926n</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Do you like them?</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8926n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1m88uxs</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>My butter yellow French tips</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q83z4f84luef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1m88nx1</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>Can't stop looking at my nails</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m88nx1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1m88fzh</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>Obsessed with this set</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m50l5s2iiuef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1m87vnt</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Loving this new set 🧡🩵</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m87vnt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1m87shh</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>Transparent nails?</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m87shh/transparent_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1m81mkk</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>How do you know if you need gel builder nails? And how do you decide acrylic versus gel nails?</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m81mkk/how_do_you_know_if_you_need_gel_builder_nails_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1m87mr4</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>The best gold glitter nail polish?</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x046xlu2duef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1m7zw8x</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>What the hell is going on</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bbrg3yivksef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1m80ku9</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>Gel that doesn't cause allergies</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m80ku9/gel_that_doesnt_cause_allergies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1m8758a</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>Did I overtrim my cuticles?</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8758a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1m862um</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>shiny heart</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hq71d2kh2uef1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1m85nn5</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>Love</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q7hn6ytgztef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1m85evh</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>Yay or nay?</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mdxmpi4qxtef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1m852c0</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>Did my nails for the first time!(gel)</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m852c0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1m85038</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>Baby pink</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m85038</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1m84xac</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>What do you think of this design? That color combination</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xxzgrfk5utef1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1m8426x</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>Faded passion red nails</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wb517cfontef1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1m839qh</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>Black French with stars</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/raaxdrljhtef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1m835vt</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>chrome-french-tip I had done in Bangkok</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m835vt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1m834fu</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>First time getting nails professionally done!</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0u5t3abrftef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1m8213s</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>Omg I love my nail tech</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xbpwhxzr6tef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1m819y2</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>Cherry nails for summer</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m819y2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1m814sv</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>Catholic nails 😍</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m814sv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1m7zoc0</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>Ditched the norm by going with Lavender instead of Red for my Indian Wedding. ✨️💜</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5e6y87xbisef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1m7z72u</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Are press-on nails reusable after I've used nail glue?</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m7z72u/are_presson_nails_reusable_after_ive_used_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1m7z63h</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>I paid $58 for this</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/24s4xxcrbsef1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1m8s4qk</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Need more Holo!</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/j6rn3su4vyef1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1m8rgma</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>Can she be saved?</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/09jegl5pnyef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1m8repz</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>Have we seen it all? Is originality still possible?</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m8repz/have_we_seen_it_all_is_originality_still_possible/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1m8pf50</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>Trying to find wolf stamps</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tvtl3ljyncef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1m8ownd</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>I attempted fruit nails (new to nail art)</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8ownd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1m8opoh</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>Had a Summer Photoshoot✨</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/87ke4ubkwxef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1m8om1v</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>LA Colors round 2</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8om1v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1m8oisn</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>I love sparkles!</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8oisn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1m8og4w</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>Stupid question, DIY scented top coat?</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m8og4w/stupid_question_diy_scented_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1m8mwwk</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>Grab Pain in the Asteroid 2.0 while you can!</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8mwwk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1m8mthv</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>Lurid Rainbow Skittle</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r3jymf2mfxef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1m8mg7n</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>Ok, you win: how do I get started with magnetics if I never tried?</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m8mg7n/ok_you_win_how_do_i_get_started_with_magnetics_if/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1m8m3rj</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>I love this thermal 😍</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8m3rj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1m8m26r</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>Irish Indie Brands!</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m8m26r/irish_indie_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1m8lxeb</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>Long time lurker, first time holographic wearer</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8lxeb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1m8lt68</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>Acrylic lifting after a week. Is it due to the application?</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m8lt68/acrylic_lifting_after_a_week_is_it_due_to_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1m8lp37</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>So many sparkles!</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/oemlohi16xef1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1m8l8qp</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>How do you all have the patience??</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m8l8qp/how_do_you_all_have_the_patience/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1m8kpz8</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>Help?</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m8kpz8/help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1m8klvy</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>Chanel rouge noir 18/ vamp</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m8klvy/chanel_rouge_noir_18_vamp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1m8klgo</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>SO BRIGHT</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nh3s1i1rwwef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1m8kldu</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>My toes are glowing</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8kldu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1m8kiz3</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>Spinning magnet over a Cirque skittle</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/q3r2i5p5wwef1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1m8juyr</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>It’s real bad isn’t it…</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8juyr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1m8js9j</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>It looks like pearls! Quo jelly "Smoke" as a base and Sinful Colors "Let me go" as a topper</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8js9j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1m8jkb3</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>A friendly PSA for other Canadian lacqueristas</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m8jkb3/a_friendly_psa_for_other_canadian_lacqueristas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1m8ixc7</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Sometimes you just have to say “screw it” and put on a known stainer</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eq6shxyljwef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1m8iab5</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>Some of my manis from the last 3 months (ft.  my nail transformation as a life long biter in remission - watch my nails grow!)</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8iab5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1m8i476</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>Easy nail designs for a beginner please !</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m8i476/easy_nail_designs_for_a_beginner_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1m8i17z</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>Can anyone find this OPI polish or somethin very similar?</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8i17z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1m8hw7d</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>Holo Taco Icon on Board</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n7ahaorobwef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1m8gwvt</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>5 Free for Gel Allergic Skin?</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m8gwvt/5_free_for_gel_allergic_skin/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1m8gexg</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>Best magnetic nails without gel?</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m8gexg/best_magnetic_nails_without_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1m8gad9</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>Does speed matter for glass bead nails?</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m8gad9/does_speed_matter_for_glass_bead_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1m8fxvf</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>Green but not mean</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ybtcafghxvef1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1m8f8gu</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>Neon, but make it holo 💿💚</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r8xdlthisvef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1m8f64g</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>1st time using Cracked and I think it might be my most favorite formula yet?</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lkbush02svef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1m8f4it</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>Excuses, excuses! (…To buy this polish)</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8f4it</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1m8ekvq</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>On mistakes in ordering sizes (to add to the Helmer vs Alex debate)</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8ekvq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1m8e5sc</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>Emily DeMolly</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fva0ch63lvef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1m8dul2</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>My new favorite polish to Velvet!</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4ycefxewivef1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1m8dd4b</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>Pokeballs :)</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9x7cw28kfvef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1m8dby1</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>I Am... a Bog Dweller</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/846xb6gbfvef1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1m8d8tq</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>Lurid: Verdant Longings and Chartreuse Memories</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8d8tq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1m8crja</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>If you need a sign to do French tips this is it.💅🏾</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qrauhz8hbvef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1m8cp6z</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>all I did was sit down at my office desk 😭</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j8hwq3t0bvef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1m8cc16</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>shooting star 💫</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/h8i61hok8vef1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1m8cbw5</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Halloween 🎃</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yub2d14h8vef1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1m8benx</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>Points Deducted for Refunds on Defective Polishes</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>/r/simplynailogical/comments/1m8bbs8/points_deducted_for_refunds_on_defective_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1m8baag</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>Then and now…</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8baag</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1m8b384</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>Atomic Polish Sour Apple Rings and Polished For Days UF-Glow</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8b384</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1m8asmi</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>looking for more look rainbow/iridescent flakie bombs</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8asmi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1m8ai66</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>Making a polish more sheer</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m8ai66/making_a_polish_more_sheer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1m89xlm</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>Uncomfortable question...</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m89xlm/uncomfortable_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1m89qk1</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>🖤🤍Dragon Fruit💚💖</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m89qk1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1m888ct</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>Emily de Molly "Oceanic Forces" 🌊</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6nlhzm45huef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1m87rq3</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>How long did it take for your paint job to start to look good?</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m87rq3/how_long_did_it_take_for_your_paint_job_to_start/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1m87o4v</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>Nails damaged from gel - Help!</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m87o4v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1m87hs6</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>When my boss asks what I've done all day, it's stare at my nails.</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wp0x8yd2cuef1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1m87fro</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>BKL Charity Mystery Magnetic ‘Heartbroken’</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7rm7om4mbuef1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1m86x32</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>Fidget spinner + magnetic polish</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dn7b67q98uef1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1m86sgn</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Baja Blasted 💥</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m86sgn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1m868b1</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>Any candids of Prism Polish: golden glade, tranquil thicket, or lividus?</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m868b1/any_candids_of_prism_polish_golden_glade_tranquil/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1m85fn5</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>Mani using entirely Craft Acrylic Paint - 1 week in, no chips!</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m85fn5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1m85dl7</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>i keep coming back to galaxies - pastel edition</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m85dl7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1m858bf</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>Danglefoot - Enth End</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kzhtkjjewtef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1m84sww</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>Didn't like this until I went out on the sun and now I'm just in love!</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tk3eaw97ttef1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1m84ovz</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>Holo Taco Wanderlust</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m84ovz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1m83tuv</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>I don't know what I did here but I like it!</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m83tuv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1m83cbf</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>Removing “waterproofed” Peely?</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zumvhth4itef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1m836vz</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>Essence cosmetics nail polishes..?</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m836vz/essence_cosmetics_nail_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1m7zboh</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>Two different colors</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dgl3w00cesef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1m7z3ol</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>Matchy-matchy</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v0tjx1c77sef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1m8ser5</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>Love this design</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kjecynq8yyef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1m8r5ia</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>My first time doing 3D cherries🍒</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ul4nhmqfkyef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1m8qb2g</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>I love flowers on my acrylic nails 🥰😍@isabellanails</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j75b8lrrbyef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1m8p4vj</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>True translucent nail chrome powders… has anyone tried any of these?</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8p4vj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1m8om8x</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Dark romance at your fingertips 💅</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ciom5fvnvxef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1m8nhxw</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>Anyone make wedding press ons?</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0up0sybolxef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1m8muu5</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>gel</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ox4h3b50gxef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1m8lh4b</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>my second pair and first time using chrome</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8lh4b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1m8jzu8</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>Uuuufffff este color tan bonito ! 😍</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p9l5jp1srwef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1m8jrsm</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>Did my own nails for the first time after watching countless YouTube videos</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8jrsm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1m8ja73</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>I made these today!</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8ja73</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1m8j1pk</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>any fantastic4 fans?</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8j1pk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1m8il3a</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>NANA inspired press-ons</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ykna5x20hwef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1m8i0zb</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>Using acrylic paint!</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8i0zb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1m8hxm9</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>Just trying some shroomies. Leaning towards no background, only mushroom.</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v9c22qlzbwef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1m8hv13</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>still very much learning but I liked the vibe of these</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ibt13ysfbwef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1m8hdrl</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>Do you like these doneby LA nails 💅</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/adno4b7u7wef1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1m8gpj0</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>mom wanted something special for her vacation 🪸🐚</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l7b23aex2wef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1m8fj09</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>What do you think of these little nails</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ep1wvojguvef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1m8ejx3</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>Some practice I did a while ago and a simple set I finished</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8ejx3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1m8dw7c</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>Today I did these nails for my mom, they turned out cute, what did you think?</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g1mgets7jvef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1m8d2kf</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>Made new flower press ons with Holo Taco Polish</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8d2kf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1m8cx4y</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>Going for an Australian Opal Vibe!!</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8cx4y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1m898fu</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>Taylor Swift Reputation-Themed Coffin Press On Set</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4qoswdgtnuef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1m88trh</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>Nails for the bad bunny residency in Puerto Rico</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tw90xjm1luef1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1m85z49</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>My Miami Nails. Made a mess with the glow powders. Used clear tips for the length.</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m85z49</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1m80jq6</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>Pokémon-Nails</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m80jq6</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Jul 26 08:11:43 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_07_27.xlsx
+++ b/data/collected_data/2025_07_27.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1126"/>
+  <dimension ref="A1:C1347"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19575,6 +19575,3763 @@
         </is>
       </c>
     </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1m9nsou</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>Oppinion about my red set</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6uwvmsezd6ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1m9neq8</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>Base of my nail came off and whatever this is is happening.</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9neq8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1m9ncqk</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>Bare Minimum - DIY Gel Nails</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m9ncqk/bare_minimum_diy_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1m9lyox</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>Sculpted acrylic set ❤️</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9lyox</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1m9l3eo</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>I keep getting infection</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j8k8ozdck5ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1m9lak6</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>What is it giving ?</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nir2rbqfm5ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1m9ks1j</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>my boyfriend said these remind him of the wiggles.</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gant6wj3h5ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1m9khmv</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>A client of my cousin</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rscsk4m6e5ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1m9jbts</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>Opinions on Nailcisist brand? Yay or Nay?</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m9jbts/opinions_on_nailcisist_brand_yay_or_nay/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1m9k4j8</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>Simple Teal and red nails</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/knr5ztona5ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1m9k44q</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>Gothy</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s0aa6xgja5ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1m9j5ld</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>Engagement nails!</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bw19c86b15ff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1m9ix55</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>Beetles nail polish and press ons</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m9ix55/beetles_nail_polish_and_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1m9ifff</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>French will never go out of style (Jojo inspo?)</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9ifff</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1m9h8od</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>I'm obsessed with chola nails</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oqy2lx0mj4ff1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1m9fbhw</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>Help!</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9fbhw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1m9iujw</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>Summer favs</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9mu40fsey4ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1m9isw0</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>Are my nails square...?</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zaa9eilyx4ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1m9io4a</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>My Dream Yellow</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/v1jcftyhw4ff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1m9igbt</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>3D Summer Nails 🍋🍋‍🟩</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9igbt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1m9idee</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>Help</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/63m7yn5yt4ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1m9hxtq</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>Warped Tour Nails</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rjncbw6xp4ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1m9hs5y</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>Haven’t done my nails in a few months… is it obvious I’m rusty?</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sopfs2yio4ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1m9hqgk</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>My new cute, short nails 🖤🐶🐱</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9hqgk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1m9hn4j</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>I always choose the color blue, I love it 💙</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p8hskfban4ff1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1m9heab</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>Sally Hansen - can't beet royal</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9heab</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1m9fm5c</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>I do my own gel overlay with jello jello peel off base coat but I feel it comes off sooner than expected</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kbhqfqtd54ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1m9fapn</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>star nails ⭐️</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9fapn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1m9f0go</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>Nail strengthening polish</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m9f0go/nail_strengthening_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1m9esry</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>3d nail gems</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fyyetm8ly3ff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1m9ecu7</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>Just sharing cause I think they're cute.</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e1m1gmu1v3ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1m9e8kg</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>celestial vibes</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aqhrfoz3u3ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1m9e5nl</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>Help! Hair keeps getting caught under press-ons when using sticky tabs</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4embcvuft3ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1m9e2ko</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>Friday salon day 😍💅🏻</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/msmj7l6rs3ff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1m9dvsv</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>Is there chrome powder i can use with non-gel polish?</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m9dvsv/is_there_chrome_powder_i_can_use_with_nongel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1m9dtej</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>Press On Sailor Moon🩷💥</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iefqan2tq3ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1m9dmy1</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>BIAB summer mani</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7z8wg1sfp3ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1m9dfjx</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>finally the way i like it,matching 🙂‍↕️</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/o4kke2psn3ff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1m9dev1</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>Purple chrome. 💜</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ubx6p6on3ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1m9d2u2</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>Acrylic removal</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jh94xet1l3ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1m9cz45</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>Some cute picnic vibes on press-ons I made today</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9cz45</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1m9cr4g</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>Very delicate</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fy4pfy6ki3ff1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1m9cqcy</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>Uñas rojas combinadas</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ggzknjqdi3ff1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1m9cgdj</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>New nails who dis 💅</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/50lhe3rcg3ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1m9bws7</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>Thoughts on super short nails</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9bws7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1m9bwi9</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>Birthday Nails! 🎂🍰🧁🎈</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9bwi9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1m9au5u</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>Are gel nails supposed to be this much hassle?</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m9au5u/are_gel_nails_supposed_to_be_this_much_hassle/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1m9ahie</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>cowboy themed “mommy &amp; me” sets</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9ahie</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1m99xwt</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>1 month of intentional nail care later.... :)</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m99xwt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1m99p1d</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>I like to match my nails to my current read🌿</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l28yo3hbw2ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1m99myz</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>Obsessed with these colors!</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m99myz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1m99g20</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>Donut nails I made</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m99g20</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1m9863p</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>Why does my top coat Bubble?</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/210i61afl2ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1m98s3v</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>Opi nail polish wont dry!</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m98s3v/opi_nail_polish_wont_dry/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1m97w0o</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>I wanted to share a set I did on myself (hobbyist)</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m97w0o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1m98hc7</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>Is the black and pink too much contrast?</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bw7k9omnn2ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1m97ymh</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>learned how to do 3d flowers!!</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vtyvic9yj2ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1m97mco</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>Decided to grow my nails out!</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m97mco</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1m97lv2</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>What do you think?</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/17kb58vdh2ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1m97hc9</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>🌊beach/pool water-effect nails!</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m97hc9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1m96s7d</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>Maybe my last set from my incredible Hungarian nail tech, and it’s for my wedding 🤍</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/20xoeklqb2ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1m96nfw</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>Friday and new design</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p500obrta2ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1m962h5</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>Added some things to my medieval inspired nails</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m962h5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1m9605g</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>Lil summer set 💛</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dbnqov6e62ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1m95w26</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>First time using builder gel. Advice? Bonus pics of old sets from clear press ons</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m95w26</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1m95lz9</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>Perfect 🪩🕺💜</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dnr2qpzp32ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1m95jzd</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>Some recent sets I did 💅🏻</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m95jzd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1m95dir</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>Kuromi nails for one of my bestie's bdays!</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m95dir</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1m94o7q</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>Brittle nails and what to tip</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m94o7q/brittle_nails_and_what_to_tip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1m94rll</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>Acrylics grew out in 3.5 weeks</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dvxyl891y1ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1m94dl5</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>Poly vs. gelx DIY</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m94dl5/poly_vs_gelx_diy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1m9435u</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>First time doing my own Gel-X</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/oizf229xs1ff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1m93sya</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Thanks for your help!!</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m93sya</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1m93nty</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>My first ombré!</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m93nty</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1m93m7f</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>Obsessed with this colour💚🌸🎀</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m93m7f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1m93hvm</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>Help with Gel Builder</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m93hvm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1m92rrm</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>Guess the inspo!</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fw4ems3mk1ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1m92y9z</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>Doing overlay on your right hand when your right handed can be challenging. What’s your hack when doing your own nails?</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x34kct0ul1ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1m92tye</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>I love this design 🌜⭐️✨️🐍🧙‍♀️</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m92tye</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1m92rgk</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>Nail update</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3eas0lvjk1ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1m92p3n</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>Natural nails :&gt;</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6vog1i24k1ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1m92nuz</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>Too old to wear fun nails?</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m92nuz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1m92l9w</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>Summer nails</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y281pydej1ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1m92igh</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>My art vs the inspo pic by @shnailz on instagram</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m92igh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1m92jyg</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>Made a simple set for now. Middle was totally freehanded</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m92jyg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1m92cwe</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>Testing press on nails to stop nail biting</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cek9agmth1ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1m92bdq</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>Mom Let Me Do a Design!</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m92bdq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1m8vrld</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>New set! :)</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8vrld</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1m8vntk</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>Nail ridges help!</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/byjhx55000ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1m8xyam</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>Help me to pick a good lamp! Question about NM!</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8xyam</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1m904b4</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>Pink Sand Beach Inspired Set 🐚🏖️</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7y4jakyd21ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1m90ma8</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>my tech did it again! 10/10</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m90ma8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1m925by</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>NANA inspired press-ons 🍓🖤</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k5faeceeg1ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1m9213u</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>Summer nails 💅🏼</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gvt19dwlf1ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1m91wl2</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>🍋🍋</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gbyuammqe1ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1m91ule</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>Cat eye nails 💅 at a Vietnamese salon in Dubai</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m91ule</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1m916ak</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>Still learning how to do my own nails</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m916ak</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1m90oud</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>mermaid nails 🧜🏼‍♀️</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vlmaloig61ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1m90kmw</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>Passionate red... I always come back to this color</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ri5130rm51ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1m90chm</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>My naturals with gel coat</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xtrgvveo31ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1m9k89l</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>1st jelly sandwich</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sl8gpwcob5ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1m9k446</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>Pink swirlies using regular polish</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9k446</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1m9jeah</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>Cirque Mood Ring</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xnpp66om35ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1m9j6ai</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>First glass bead experiment + Dog tax</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/skviavwh15ff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1m9duf9</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>First post: July Manis</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9duf9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1m9h6ze</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>EdM hit it out of the park!</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9h6ze</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1m9i4pr</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>My first ever Cracked haul arrived today!</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9i4pr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1m9i4d2</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>Shiny</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6dt94c2mr4ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1m9hriz</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>Windchime Spinner</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1r2n0jp9n4ff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1m9h15i</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>“Why polished_mustelid?” My life:</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1cy2ghsoh4ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1m9gdox</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>more bg3 polishes please</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9gdox</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1m9g5hd</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>Retail therapy in this economy?</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7mz3r4rx94ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1m9fiv2</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>Unhinged apple swatches</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9fiv2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1m9fftt</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>I don't normally wear one polish on my left hand, but when I do it's actually 12 polishes.</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9fftt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1m9fd1h</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>Tea light 🕯️</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6edpz4n834ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1m9f736</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>Black &amp; floral, black &amp; floral (to the tune of wiz khalifa)</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9f736</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1m9eq5q</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>Mother of Pearl Nails</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9eq5q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1m9egj6</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>It’s growing on me</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nugqcdxvv3ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1m9do46</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>ILNP Cityscape</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9do46</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1m9d8f0</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>ILNP in the sun</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9d8f0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1m9d3z8</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>Your holy-grail base coats?</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m9d3z8/your_holygrail_base_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1m9csdd</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>Recreated the froggy 🐸💙</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9csdd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1m9cn3x</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>I can do a simple nail art mani faster than a full magnetic set, right? RIGHT?</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9cn3x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1m9ckpx</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>Magnetics spreading/fading hours after application?</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m9ckpx/magnetics_spreadingfading_hours_after_application/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1m956dw</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>My second attempt at gel nails at home - is the gel layer too thin? How do they look?</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m956dw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1m8msru</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>Any blood red nail polish recommendations?</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m8msru/any_blood_red_nail_polish_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1m9c0gd</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>(None dominant hand not pictured for obvious reasons) + kitty tax</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9c0gd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1m9bzpb</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>L.A. Colors appreciation.</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9bzpb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1m9bwzv</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>Flower Child over Gunmetal</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vp8522ccc3ff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1m9bkp6</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>Rogue Lacquer - Lincoln Park Lush</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/te1jhqxs93ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1m9bait</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>I like MoonCat’s Pandemonium BECAUSE it looks orange!</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9bait</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1m9b943</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>Love this one</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dbnrm8zd73ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1m9ayw4</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>Peachy Keen</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9ayw4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1m9alsg</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>Topcoat Thickness A/B Test Results!</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9alsg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1m9acow</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>Nail Cleaner</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m9acow/nail_cleaner/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1m9aaq7</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>Lurid Lacquer  “You Survived”</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9aaq7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1m9aaex</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>What a Pearl Wants</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9aaex</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1m9a30a</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>Nail brush cleaner?</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m9a30a/nail_brush_cleaner/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1m99zva</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>I didn’t know anything about magnets and imperial units so i accidentally bought a REALLY strong magnet</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m99zva/i_didnt_know_anything_about_magnets_and_imperial/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1m99yum</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>Dray Hand Care</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m99yum</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1m99tce</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>More hype for Wanderlust please!</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m99tce</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1m99sxs</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>Growing out the nails again...</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aq4sc7s3x2ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1m99p3o</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>I guess I’m falling in love with pink</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e8p84hvbw2ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1m99lfk</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>Lurid: Morus Alba, My Foe</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m99lfk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1m99ctp</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>Milky Wave🩵</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m99ctp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1m990a5</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>Hi friends, I’m doing an official mooncat giveaway over on YouTube 🐈‍⬛</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m990a5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1m98x06</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>Any recommendations for artist in paris?</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m98x06</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1m97k0h</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>A little magnetic ocean</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6obm1sw3h2ff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1m97jvs</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>Poolside Nails 🌊 Cat-eye water effect</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m97jvs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1m97brx</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>A pleasant surprise</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m97brx/a_pleasant_surprise/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1m977g6</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>Last July manicure.</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m977g6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1m96lvx</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>cirque “pele”</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m96lvx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1m9649i</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>We're going to need a big magnet. 🦈 week mani!</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9649i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1m95gv4</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>Wearing bluebell on vacation</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m95gv4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1m95epd</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>Gunmetal for warm tones 🥳</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xqp3ckhc22ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1m957xd</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>Lurid - One Bite For Me 🍉</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ch759gm212ff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1m954m3</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>Sent this text to my husband and to his credit he *almost* understood it. How many laquerista subculture terms can you fit in one sentence? 😆</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a8vlf6sg02ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1m94w8b</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>loveee this one</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m94w8b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1m94s83</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>Poly vs. gelx DIY</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>/r/Nails/comments/1m94dl5/poly_vs_gelx_diy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1m94s5c</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>searching for yellows</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8dae0wx4y1ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1m94qx5</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>Rogue lacquer Ocean Water</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/m4098vsux1ff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1m94lud</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>When the layering experiment is a success</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/be13lgezw1ff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1m945xc</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>Brands with the best multichromes</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m945xc/brands_with_the_best_multichromes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1m9435m</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>made my first set of press ons!!!</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9435m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1m940zv</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>Pink Lemonade is crazy</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/q85hy842t1ff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1m93z4i</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>I’m sorry, Rum Ham!!!</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m93z4i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1m93j74</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>Bright flakies for summer? How groundbreaking!</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g7s5v0mpp1ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1m93ct8</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>First time sharing my mani here</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/orbedyd8o1ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1m93b8b</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>Nail repair kit before or after polishing?</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m93b8b/nail_repair_kit_before_or_after_polishing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1m92yws</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>mooncat - welcome to paradise - diff lighting (gifted pr)</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/aun8zvfxl1ff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1m92ra9</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>Favorite food inspired polishes?</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m92ra9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1m9212z</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>Indomitable, two ways</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9212z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1m91h61</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>30lb vs 20lb Magnet: A Better Comparison</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ifyc2d8vb1ff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1m91czb</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>Life hack: when your polish shafts to chip off, instead of touching it up, just trim your nails down! /s</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m91czb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1m91a0n</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>Game changer to prevent skin picking? I trimmed my index fingernails!</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/utyagr3ha1ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1m9158j</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>Opi - Hi Ken!</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g0wmrrhk91ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1m90zqd</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>Are there any polishes that look like Dita Von Teese's wedding dress? (Red/blue/purple shift)</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m90zqd/are_there_any_polishes_that_look_like_dita_von/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1m90zdy</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>i may have slightly overshot “cool and chic” and accidentally gave myself “6 week grow out” instead 🥴</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m90zdy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1m90q3e</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>🍣Sushi Nails🍣</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m90q3e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1m908m4</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>Drying magnetic polish</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m908m4/drying_magnetic_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1m901qi</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>Read Between My Tulips is STUNNING</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m901qi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1m8zk0u</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>Nail Color for Daughter's Wedding</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ncyzch79y0ff1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1m8ze2s</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>Stained Glass Nails</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ybxz3p91w0ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1m8ygku</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>Lurid Lacquer The Polish Mage</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8ygku</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1m8y1jc</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>Tips on how to paint these tips?</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sd2amqpfm0ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1m8xnwv</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>A Formula 1 Themed Skittle Mani</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ikx6ss68j0ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1m8x40p</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>Vintage Sinful Colours - Ecuador</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7t41oq46e0ff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1m8ww8y</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>ILNP Glowstick vs Flower Child</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8ww8y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1m8wlto</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>Highly requested comparison, thought I would share here.</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g4yqrxhn90ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1m8wfu8</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>Such a juicy soft pink</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8wfu8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1m8vj1v</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>Wanted an excuse to use my new Holo Taco 🌮</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lkexs47jyzef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1m8vgrl</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>Fun with stamping 🧡💜</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hjcddsytxzef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1m8tj11</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>What are the craziest polish names you’ve come across?</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nap62c99bzef1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1m9mvan</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>Best 3D gel in a pot (not a squeeze tube)</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1m9mvan/best_3d_gel_in_a_pot_not_a_squeeze_tube/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1m9m4ob</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>Fruity fresh and fun for summer</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i17v937su5ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1m9kld4</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>Late night post - freestyle set</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9kld4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1m9jeoo</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>Hello Kitty</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9jeoo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1m9ifyr</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>Timeless French tips... Jojo, anyone?</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9ifyr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1m9hugh</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>Here’s how to get the perfect seashell nails 🐚💅</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/63rsyfz2p4ff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1m9hr74</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>Nails pink 🩷</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xicf0xhao4ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1m9g7sb</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>Fruit slices and other things!</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9g7sb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1m9g17x</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>Me encanta cuando las clientas me ponen a prueba !</t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9g17x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1m9fyil</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t>Second time painting my nails, I love how they turned out!! Still learning how to use gel</t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qh7ricga84ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t>1m9fs07</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t>spongebob nails!</t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9vmohg4p64ff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>1m9dkky</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>Handpainted Peterson and Findus art on natural nails</t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9dkky</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>1m9d70i</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>Fav pose so far</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9d70i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t>1m9c4qn</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t>I can’t tell if these nails are cute or not</t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qtmakteyd3ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t>1m9bx81</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t>Some of my favorites from this year</t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9bx81</t>
+        </is>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t>1m9ayvs</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t>geo nail polish recommendations (for a beginner!)</t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9ayvs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr">
+        <is>
+          <t>1m9akok</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t>Some funky bugs I did today!</t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9akok</t>
+        </is>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr">
+        <is>
+          <t>1m9af8g</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t>cowboy themed “mommy &amp; me” press-on set</t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9af8g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr">
+        <is>
+          <t>1m99sw0</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t>ICE CREAM NAILS 🍨</t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nhggv783x2ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr">
+        <is>
+          <t>1m98x69</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t>✨</t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m98x69</t>
+        </is>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr">
+        <is>
+          <t>1m97zse</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t>tropical set !</t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8xa5eco6k2ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr">
+        <is>
+          <t>1m97jdp</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t>My neighbor totoro</t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m97jdp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr">
+        <is>
+          <t>1m960lg</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t>My most recent set on myself</t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m960lg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" t="inlineStr">
+        <is>
+          <t>1m95kz0</t>
+        </is>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t>Some recent sets I did 💅🏻</t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m95kz0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" t="inlineStr">
+        <is>
+          <t>1m950mz</t>
+        </is>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t>Almost died (it’s too hot where I am now and the 3d gel was behaving like a regular builder)</t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/i6iud3fvy1ff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" t="inlineStr">
+        <is>
+          <t>1m92n9l</t>
+        </is>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t>Marble nails</t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m92n9l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" t="inlineStr">
+        <is>
+          <t>1m8zjbc</t>
+        </is>
+      </c>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t>Fresh and Juicy</t>
+        </is>
+      </c>
+      <c r="C1346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m8zjbc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" t="inlineStr">
+        <is>
+          <t>1m90cm3</t>
+        </is>
+      </c>
+      <c r="B1347" t="inlineStr">
+        <is>
+          <t>Second set ever</t>
+        </is>
+      </c>
+      <c r="C1347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m90cm3</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Jul 27 08:11:47 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_07_27.xlsx
+++ b/data/collected_data/2025_07_27.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1347"/>
+  <dimension ref="A1:C1556"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -23332,6 +23332,3559 @@
         </is>
       </c>
     </row>
+    <row r="1348">
+      <c r="A1348" t="inlineStr">
+        <is>
+          <t>1maguy5</t>
+        </is>
+      </c>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t>Best gel polish brands in the EU?</t>
+        </is>
+      </c>
+      <c r="C1348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1maguy5/best_gel_polish_brands_in_the_eu/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" t="inlineStr">
+        <is>
+          <t>1mafeoz</t>
+        </is>
+      </c>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t>set i did on myself awhile ago, just never got to share</t>
+        </is>
+      </c>
+      <c r="C1349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mafeoz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" t="inlineStr">
+        <is>
+          <t>1maebtq</t>
+        </is>
+      </c>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t>I put no wipe top coat on top of chrome, is that why it’s peeling?</t>
+        </is>
+      </c>
+      <c r="C1350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1maebtq/i_put_no_wipe_top_coat_on_top_of_chrome_is_that/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" t="inlineStr">
+        <is>
+          <t>1macmwt</t>
+        </is>
+      </c>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t>Get these off of me!!!</t>
+        </is>
+      </c>
+      <c r="C1351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1macmwt/get_these_off_of_me/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1352">
+      <c r="A1352" t="inlineStr">
+        <is>
+          <t>1maeu7u</t>
+        </is>
+      </c>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t>Showing off 🫶🏻</t>
+        </is>
+      </c>
+      <c r="C1352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1maeu7u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" t="inlineStr">
+        <is>
+          <t>1maei88</t>
+        </is>
+      </c>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t>nails, labubu, and Beyoncé!!</t>
+        </is>
+      </c>
+      <c r="C1353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nfcejjeqtcff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1354">
+      <c r="A1354" t="inlineStr">
+        <is>
+          <t>1maehps</t>
+        </is>
+      </c>
+      <c r="B1354" t="inlineStr">
+        <is>
+          <t>New nailsssss peep the koi fish!</t>
+        </is>
+      </c>
+      <c r="C1354" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ygdlzb2ltcff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1355">
+      <c r="A1355" t="inlineStr">
+        <is>
+          <t>1madtzq</t>
+        </is>
+      </c>
+      <c r="B1355" t="inlineStr">
+        <is>
+          <t>Gel top coat - keeping it clean</t>
+        </is>
+      </c>
+      <c r="C1355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1madtzq/gel_top_coat_keeping_it_clean/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1356">
+      <c r="A1356" t="inlineStr">
+        <is>
+          <t>1maczqu</t>
+        </is>
+      </c>
+      <c r="B1356" t="inlineStr">
+        <is>
+          <t>Prep help!!!</t>
+        </is>
+      </c>
+      <c r="C1356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1maczqu/prep_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1357">
+      <c r="A1357" t="inlineStr">
+        <is>
+          <t>1madfki</t>
+        </is>
+      </c>
+      <c r="B1357" t="inlineStr">
+        <is>
+          <t>Wire wrapped opals🤍</t>
+        </is>
+      </c>
+      <c r="C1357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1madfki</t>
+        </is>
+      </c>
+    </row>
+    <row r="1358">
+      <c r="A1358" t="inlineStr">
+        <is>
+          <t>1madjvl</t>
+        </is>
+      </c>
+      <c r="B1358" t="inlineStr">
+        <is>
+          <t>my first time doing nails!!</t>
+        </is>
+      </c>
+      <c r="C1358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1madjvl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1359">
+      <c r="A1359" t="inlineStr">
+        <is>
+          <t>1madimg</t>
+        </is>
+      </c>
+      <c r="B1359" t="inlineStr">
+        <is>
+          <t>Perfect</t>
+        </is>
+      </c>
+      <c r="C1359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9den1hd7jcff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1360">
+      <c r="A1360" t="inlineStr">
+        <is>
+          <t>1mad6s2</t>
+        </is>
+      </c>
+      <c r="B1360" t="inlineStr">
+        <is>
+          <t>in purple</t>
+        </is>
+      </c>
+      <c r="C1360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g7kdyi2ufcff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1361">
+      <c r="A1361" t="inlineStr">
+        <is>
+          <t>1macyf1</t>
+        </is>
+      </c>
+      <c r="B1361" t="inlineStr">
+        <is>
+          <t>new set 💚</t>
+        </is>
+      </c>
+      <c r="C1361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1macyf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1362">
+      <c r="A1362" t="inlineStr">
+        <is>
+          <t>1macuuw</t>
+        </is>
+      </c>
+      <c r="B1362" t="inlineStr">
+        <is>
+          <t>Are there temporary nails that I can remove on my own?</t>
+        </is>
+      </c>
+      <c r="C1362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1macuuw/are_there_temporary_nails_that_i_can_remove_on_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1363">
+      <c r="A1363" t="inlineStr">
+        <is>
+          <t>1macqlz</t>
+        </is>
+      </c>
+      <c r="B1363" t="inlineStr">
+        <is>
+          <t>new nails! i learned to do my own around January of this year and Im not sure if I have any bad habits I’m not seeing on my nails.</t>
+        </is>
+      </c>
+      <c r="C1363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1macqlz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1364">
+      <c r="A1364" t="inlineStr">
+        <is>
+          <t>1maceqq</t>
+        </is>
+      </c>
+      <c r="B1364" t="inlineStr">
+        <is>
+          <t>Everyone keeps complimenting my nails</t>
+        </is>
+      </c>
+      <c r="C1364" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1zggszn48cff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1365">
+      <c r="A1365" t="inlineStr">
+        <is>
+          <t>1mac5of</t>
+        </is>
+      </c>
+      <c r="B1365" t="inlineStr">
+        <is>
+          <t>Care Bear themed nails</t>
+        </is>
+      </c>
+      <c r="C1365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mac5of</t>
+        </is>
+      </c>
+    </row>
+    <row r="1366">
+      <c r="A1366" t="inlineStr">
+        <is>
+          <t>1ma5qq3</t>
+        </is>
+      </c>
+      <c r="B1366" t="inlineStr">
+        <is>
+          <t>Getting into abstract designs</t>
+        </is>
+      </c>
+      <c r="C1366" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lj6w38pwkaff1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1367">
+      <c r="A1367" t="inlineStr">
+        <is>
+          <t>1ma5xot</t>
+        </is>
+      </c>
+      <c r="B1367" t="inlineStr">
+        <is>
+          <t>My poor toenail</t>
+        </is>
+      </c>
+      <c r="C1367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ma5xot</t>
+        </is>
+      </c>
+    </row>
+    <row r="1368">
+      <c r="A1368" t="inlineStr">
+        <is>
+          <t>1ma6o52</t>
+        </is>
+      </c>
+      <c r="B1368" t="inlineStr">
+        <is>
+          <t>Any idea what's happening with this polish?</t>
+        </is>
+      </c>
+      <c r="C1368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ma6o52</t>
+        </is>
+      </c>
+    </row>
+    <row r="1369">
+      <c r="A1369" t="inlineStr">
+        <is>
+          <t>1maawm2</t>
+        </is>
+      </c>
+      <c r="B1369" t="inlineStr">
+        <is>
+          <t>Dip manicure help</t>
+        </is>
+      </c>
+      <c r="C1369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1maawm2/dip_manicure_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1370">
+      <c r="A1370" t="inlineStr">
+        <is>
+          <t>1mabkcz</t>
+        </is>
+      </c>
+      <c r="B1370" t="inlineStr">
+        <is>
+          <t>i love my new hobby</t>
+        </is>
+      </c>
+      <c r="C1370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mabkcz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1371">
+      <c r="A1371" t="inlineStr">
+        <is>
+          <t>1mab7b0</t>
+        </is>
+      </c>
+      <c r="B1371" t="inlineStr">
+        <is>
+          <t>Do nail salons glue nails back on</t>
+        </is>
+      </c>
+      <c r="C1371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mab7b0/do_nail_salons_glue_nails_back_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1372">
+      <c r="A1372" t="inlineStr">
+        <is>
+          <t>1mab1ti</t>
+        </is>
+      </c>
+      <c r="B1372" t="inlineStr">
+        <is>
+          <t>I just like pretty rocks…</t>
+        </is>
+      </c>
+      <c r="C1372" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g51oku88vbff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1373">
+      <c r="A1373" t="inlineStr">
+        <is>
+          <t>1maasfu</t>
+        </is>
+      </c>
+      <c r="B1373" t="inlineStr">
+        <is>
+          <t>One of my latest works, I love red! And the red cat eye more 🤣🫶🏻</t>
+        </is>
+      </c>
+      <c r="C1373" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p7ejs6jssbff1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1374">
+      <c r="A1374" t="inlineStr">
+        <is>
+          <t>1maanmx</t>
+        </is>
+      </c>
+      <c r="B1374" t="inlineStr">
+        <is>
+          <t>First time doing GelX on myself</t>
+        </is>
+      </c>
+      <c r="C1374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1maanmx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1375">
+      <c r="A1375" t="inlineStr">
+        <is>
+          <t>1maafr9</t>
+        </is>
+      </c>
+      <c r="B1375" t="inlineStr">
+        <is>
+          <t>Blooming gel 🌸</t>
+        </is>
+      </c>
+      <c r="C1375" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5gdaca4ppbff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1376">
+      <c r="A1376" t="inlineStr">
+        <is>
+          <t>1ma9tbo</t>
+        </is>
+      </c>
+      <c r="B1376" t="inlineStr">
+        <is>
+          <t>Birthday nails babyyy</t>
+        </is>
+      </c>
+      <c r="C1376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ma9tbo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1377">
+      <c r="A1377" t="inlineStr">
+        <is>
+          <t>1ma9oe9</t>
+        </is>
+      </c>
+      <c r="B1377" t="inlineStr">
+        <is>
+          <t>First Attempt At Gel Nails</t>
+        </is>
+      </c>
+      <c r="C1377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ma9oe9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1378">
+      <c r="A1378" t="inlineStr">
+        <is>
+          <t>1ma9dq1</t>
+        </is>
+      </c>
+      <c r="B1378" t="inlineStr">
+        <is>
+          <t>Super simple for my 3rd set. A nod to my favourite kpop group Blackpink 🥰🖤🩷</t>
+        </is>
+      </c>
+      <c r="C1378" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/romndx81gbff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1379">
+      <c r="A1379" t="inlineStr">
+        <is>
+          <t>1ma97bh</t>
+        </is>
+      </c>
+      <c r="B1379" t="inlineStr">
+        <is>
+          <t>Jello Jello Peel off base</t>
+        </is>
+      </c>
+      <c r="C1379" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cuw7qldfebff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1380">
+      <c r="A1380" t="inlineStr">
+        <is>
+          <t>1ma9267</t>
+        </is>
+      </c>
+      <c r="B1380" t="inlineStr">
+        <is>
+          <t>what color should i put under this to make a somewhat shiny vibrant teal? (i dont have teal)</t>
+        </is>
+      </c>
+      <c r="C1380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ma9267</t>
+        </is>
+      </c>
+    </row>
+    <row r="1381">
+      <c r="A1381" t="inlineStr">
+        <is>
+          <t>1ma8x67</t>
+        </is>
+      </c>
+      <c r="B1381" t="inlineStr">
+        <is>
+          <t>Lavender Nails</t>
+        </is>
+      </c>
+      <c r="C1381" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i5oygsmwbbff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1382">
+      <c r="A1382" t="inlineStr">
+        <is>
+          <t>1ma8r60</t>
+        </is>
+      </c>
+      <c r="B1382" t="inlineStr">
+        <is>
+          <t>My first time ever doing my nails at a salon! What do you think?</t>
+        </is>
+      </c>
+      <c r="C1382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ma8r60</t>
+        </is>
+      </c>
+    </row>
+    <row r="1383">
+      <c r="A1383" t="inlineStr">
+        <is>
+          <t>1ma8j8o</t>
+        </is>
+      </c>
+      <c r="B1383" t="inlineStr">
+        <is>
+          <t>Raspberry Ripple</t>
+        </is>
+      </c>
+      <c r="C1383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ma8j8o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1384">
+      <c r="A1384" t="inlineStr">
+        <is>
+          <t>1ma8c8t</t>
+        </is>
+      </c>
+      <c r="B1384" t="inlineStr">
+        <is>
+          <t>Customized press ons myself, purrrrr 🐱 🎀 💅🏾</t>
+        </is>
+      </c>
+      <c r="C1384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ma8c8t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1385">
+      <c r="A1385" t="inlineStr">
+        <is>
+          <t>1ma849v</t>
+        </is>
+      </c>
+      <c r="B1385" t="inlineStr">
+        <is>
+          <t>First time doing a gel French tip</t>
+        </is>
+      </c>
+      <c r="C1385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ma849v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1386">
+      <c r="A1386" t="inlineStr">
+        <is>
+          <t>1ma844w</t>
+        </is>
+      </c>
+      <c r="B1386" t="inlineStr">
+        <is>
+          <t>what shape would best suit me</t>
+        </is>
+      </c>
+      <c r="C1386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/82gn7qvo4bff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1387">
+      <c r="A1387" t="inlineStr">
+        <is>
+          <t>1ma7tl1</t>
+        </is>
+      </c>
+      <c r="B1387" t="inlineStr">
+        <is>
+          <t>A little citrus for summer!</t>
+        </is>
+      </c>
+      <c r="C1387" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q8sw8sr32bff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1388">
+      <c r="A1388" t="inlineStr">
+        <is>
+          <t>1ma7qqa</t>
+        </is>
+      </c>
+      <c r="B1388" t="inlineStr">
+        <is>
+          <t>Just a reminder to be careful with acrylic nails!!</t>
+        </is>
+      </c>
+      <c r="C1388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ma7qqa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1389">
+      <c r="A1389" t="inlineStr">
+        <is>
+          <t>1ma7oz2</t>
+        </is>
+      </c>
+      <c r="B1389" t="inlineStr">
+        <is>
+          <t>Sally Hansen - tangerine dream</t>
+        </is>
+      </c>
+      <c r="C1389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ma7oz2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1390">
+      <c r="A1390" t="inlineStr">
+        <is>
+          <t>1ma7gvj</t>
+        </is>
+      </c>
+      <c r="B1390" t="inlineStr">
+        <is>
+          <t>Acrylic, dip, other options? What’s best</t>
+        </is>
+      </c>
+      <c r="C1390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ma7gvj/acrylic_dip_other_options_whats_best/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1391">
+      <c r="A1391" t="inlineStr">
+        <is>
+          <t>1ma7esd</t>
+        </is>
+      </c>
+      <c r="B1391" t="inlineStr">
+        <is>
+          <t>summer gradient 🧡🩷</t>
+        </is>
+      </c>
+      <c r="C1391" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rxz7hjsgyaff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1392">
+      <c r="A1392" t="inlineStr">
+        <is>
+          <t>1ma7a6l</t>
+        </is>
+      </c>
+      <c r="B1392" t="inlineStr">
+        <is>
+          <t>my new nails today</t>
+        </is>
+      </c>
+      <c r="C1392" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4v06aqojxaff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1393">
+      <c r="A1393" t="inlineStr">
+        <is>
+          <t>1ma78pw</t>
+        </is>
+      </c>
+      <c r="B1393" t="inlineStr">
+        <is>
+          <t>Complete noob</t>
+        </is>
+      </c>
+      <c r="C1393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ma78pw/complete_noob/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1394">
+      <c r="A1394" t="inlineStr">
+        <is>
+          <t>1ma746c</t>
+        </is>
+      </c>
+      <c r="B1394" t="inlineStr">
+        <is>
+          <t>My last and current set ❤️🤍🖤</t>
+        </is>
+      </c>
+      <c r="C1394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ma746c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1395">
+      <c r="A1395" t="inlineStr">
+        <is>
+          <t>1ma6mw0</t>
+        </is>
+      </c>
+      <c r="B1395" t="inlineStr">
+        <is>
+          <t>Basic set, but best set I’ve had in a while!</t>
+        </is>
+      </c>
+      <c r="C1395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ma6mw0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1396">
+      <c r="A1396" t="inlineStr">
+        <is>
+          <t>1ma6hdd</t>
+        </is>
+      </c>
+      <c r="B1396" t="inlineStr">
+        <is>
+          <t>This nail needs help</t>
+        </is>
+      </c>
+      <c r="C1396" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jvqg9civqaff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1397">
+      <c r="A1397" t="inlineStr">
+        <is>
+          <t>1ma6a52</t>
+        </is>
+      </c>
+      <c r="B1397" t="inlineStr">
+        <is>
+          <t>Custom press on orders of the week✨💅🏼☁️💕</t>
+        </is>
+      </c>
+      <c r="C1397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ma6a52</t>
+        </is>
+      </c>
+    </row>
+    <row r="1398">
+      <c r="A1398" t="inlineStr">
+        <is>
+          <t>1ma60mf</t>
+        </is>
+      </c>
+      <c r="B1398" t="inlineStr">
+        <is>
+          <t>Pedicure for a partial toenail</t>
+        </is>
+      </c>
+      <c r="C1398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ma60mf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1399">
+      <c r="A1399" t="inlineStr">
+        <is>
+          <t>1ma5upb</t>
+        </is>
+      </c>
+      <c r="B1399" t="inlineStr">
+        <is>
+          <t>Abstract isolated chrome with cat eye</t>
+        </is>
+      </c>
+      <c r="C1399" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tocvotaslaff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1400">
+      <c r="A1400" t="inlineStr">
+        <is>
+          <t>1ma5pq1</t>
+        </is>
+      </c>
+      <c r="B1400" t="inlineStr">
+        <is>
+          <t>What do you think of this design?</t>
+        </is>
+      </c>
+      <c r="C1400" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2v8yhccokaff1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1401">
+      <c r="A1401" t="inlineStr">
+        <is>
+          <t>1ma5ntv</t>
+        </is>
+      </c>
+      <c r="B1401" t="inlineStr">
+        <is>
+          <t>Fs in the chat…</t>
+        </is>
+      </c>
+      <c r="C1401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o0l0h347kaff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1402">
+      <c r="A1402" t="inlineStr">
+        <is>
+          <t>1ma5mty</t>
+        </is>
+      </c>
+      <c r="B1402" t="inlineStr">
+        <is>
+          <t>birthday nails 🥰</t>
+        </is>
+      </c>
+      <c r="C1402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ma5mty</t>
+        </is>
+      </c>
+    </row>
+    <row r="1403">
+      <c r="A1403" t="inlineStr">
+        <is>
+          <t>1ma5hvy</t>
+        </is>
+      </c>
+      <c r="B1403" t="inlineStr">
+        <is>
+          <t>Fresh set!</t>
+        </is>
+      </c>
+      <c r="C1403" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nlkhppd0jaff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1404">
+      <c r="A1404" t="inlineStr">
+        <is>
+          <t>1ma5av9</t>
+        </is>
+      </c>
+      <c r="B1404" t="inlineStr">
+        <is>
+          <t>Sparkly nails</t>
+        </is>
+      </c>
+      <c r="C1404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ma5av9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1405">
+      <c r="A1405" t="inlineStr">
+        <is>
+          <t>1ma4ym5</t>
+        </is>
+      </c>
+      <c r="B1405" t="inlineStr">
+        <is>
+          <t>Watermelon, blushed, cat-eye, summer press on set</t>
+        </is>
+      </c>
+      <c r="C1405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ma4ym5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1406">
+      <c r="A1406" t="inlineStr">
+        <is>
+          <t>1ma4xyd</t>
+        </is>
+      </c>
+      <c r="B1406" t="inlineStr">
+        <is>
+          <t>Pretty in pink..</t>
+        </is>
+      </c>
+      <c r="C1406" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ez0jruqeaff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1407">
+      <c r="A1407" t="inlineStr">
+        <is>
+          <t>1ma4xin</t>
+        </is>
+      </c>
+      <c r="B1407" t="inlineStr">
+        <is>
+          <t>Second time doing nail art!t</t>
+        </is>
+      </c>
+      <c r="C1407" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y6c8d0gneaff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1408">
+      <c r="A1408" t="inlineStr">
+        <is>
+          <t>1ma4fng</t>
+        </is>
+      </c>
+      <c r="B1408" t="inlineStr">
+        <is>
+          <t>new nails before my birthday!</t>
+        </is>
+      </c>
+      <c r="C1408" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6dk6mr0taaff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1409">
+      <c r="A1409" t="inlineStr">
+        <is>
+          <t>1ma3wyj</t>
+        </is>
+      </c>
+      <c r="B1409" t="inlineStr">
+        <is>
+          <t>So Happy how they Turned out!</t>
+        </is>
+      </c>
+      <c r="C1409" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6j3izdeq6aff1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1410">
+      <c r="A1410" t="inlineStr">
+        <is>
+          <t>1ma3wb6</t>
+        </is>
+      </c>
+      <c r="B1410" t="inlineStr">
+        <is>
+          <t>Helppp😭</t>
+        </is>
+      </c>
+      <c r="C1410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ma3wb6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1411">
+      <c r="A1411" t="inlineStr">
+        <is>
+          <t>1ma3tkc</t>
+        </is>
+      </c>
+      <c r="B1411" t="inlineStr">
+        <is>
+          <t>F1/McLaren themed nails, ready for the Hungarian GP next week 🧡🏎</t>
+        </is>
+      </c>
+      <c r="C1411" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/leg8mol46aff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1412">
+      <c r="A1412" t="inlineStr">
+        <is>
+          <t>1ma33aw</t>
+        </is>
+      </c>
+      <c r="B1412" t="inlineStr">
+        <is>
+          <t>How long do you guys usually take to do a fill?</t>
+        </is>
+      </c>
+      <c r="C1412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ma33aw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1413">
+      <c r="A1413" t="inlineStr">
+        <is>
+          <t>1m9skae</t>
+        </is>
+      </c>
+      <c r="B1413" t="inlineStr">
+        <is>
+          <t>What do I ask for?</t>
+        </is>
+      </c>
+      <c r="C1413" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vdmnwzwlt7ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1414">
+      <c r="A1414" t="inlineStr">
+        <is>
+          <t>1ma3fyr</t>
+        </is>
+      </c>
+      <c r="B1414" t="inlineStr">
+        <is>
+          <t>Is it okay to do gel every day?</t>
+        </is>
+      </c>
+      <c r="C1414" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rn7siil93aff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1415">
+      <c r="A1415" t="inlineStr">
+        <is>
+          <t>1ma38pe</t>
+        </is>
+      </c>
+      <c r="B1415" t="inlineStr">
+        <is>
+          <t>Halloween Nails</t>
+        </is>
+      </c>
+      <c r="C1415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ma38pe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1416">
+      <c r="A1416" t="inlineStr">
+        <is>
+          <t>1ma381p</t>
+        </is>
+      </c>
+      <c r="B1416" t="inlineStr">
+        <is>
+          <t>Flexing my nails</t>
+        </is>
+      </c>
+      <c r="C1416" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/66lspzmk1aff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1417">
+      <c r="A1417" t="inlineStr">
+        <is>
+          <t>1ma2943</t>
+        </is>
+      </c>
+      <c r="B1417" t="inlineStr">
+        <is>
+          <t>new nails 💅</t>
+        </is>
+      </c>
+      <c r="C1417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ma2943</t>
+        </is>
+      </c>
+    </row>
+    <row r="1418">
+      <c r="A1418" t="inlineStr">
+        <is>
+          <t>1ma0x6t</t>
+        </is>
+      </c>
+      <c r="B1418" t="inlineStr">
+        <is>
+          <t>This is bulky, right ?</t>
+        </is>
+      </c>
+      <c r="C1418" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hcnftr8ck9ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1419">
+      <c r="A1419" t="inlineStr">
+        <is>
+          <t>1ma1k31</t>
+        </is>
+      </c>
+      <c r="B1419" t="inlineStr">
+        <is>
+          <t>Love my nail tech</t>
+        </is>
+      </c>
+      <c r="C1419" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fkz8wpf1p9ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1420">
+      <c r="A1420" t="inlineStr">
+        <is>
+          <t>1ma1aq8</t>
+        </is>
+      </c>
+      <c r="B1420" t="inlineStr">
+        <is>
+          <t>Loving the summer fruits!</t>
+        </is>
+      </c>
+      <c r="C1420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ma1aq8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1421">
+      <c r="A1421" t="inlineStr">
+        <is>
+          <t>1ma10rh</t>
+        </is>
+      </c>
+      <c r="B1421" t="inlineStr">
+        <is>
+          <t>Quartz 💎 💅  (beginner)</t>
+        </is>
+      </c>
+      <c r="C1421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ma10rh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1422">
+      <c r="A1422" t="inlineStr">
+        <is>
+          <t>1ma0kb1</t>
+        </is>
+      </c>
+      <c r="B1422" t="inlineStr">
+        <is>
+          <t>Just a simple cityscape. First of 10. Ferris wheel up next!</t>
+        </is>
+      </c>
+      <c r="C1422" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zuhzcwltg9ff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1423">
+      <c r="A1423" t="inlineStr">
+        <is>
+          <t>1ma0k4i</t>
+        </is>
+      </c>
+      <c r="B1423" t="inlineStr">
+        <is>
+          <t>Apex?</t>
+        </is>
+      </c>
+      <c r="C1423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ma0k4i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1424">
+      <c r="A1424" t="inlineStr">
+        <is>
+          <t>1ma0ef5</t>
+        </is>
+      </c>
+      <c r="B1424" t="inlineStr">
+        <is>
+          <t>5 shades of pink</t>
+        </is>
+      </c>
+      <c r="C1424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ma0ef5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1425">
+      <c r="A1425" t="inlineStr">
+        <is>
+          <t>1ma0cod</t>
+        </is>
+      </c>
+      <c r="B1425" t="inlineStr">
+        <is>
+          <t>Some of my favorite work from the nail salon!</t>
+        </is>
+      </c>
+      <c r="C1425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ma0cod</t>
+        </is>
+      </c>
+    </row>
+    <row r="1426">
+      <c r="A1426" t="inlineStr">
+        <is>
+          <t>1ma0c5t</t>
+        </is>
+      </c>
+      <c r="B1426" t="inlineStr">
+        <is>
+          <t>Queen Brand Glow Gel</t>
+        </is>
+      </c>
+      <c r="C1426" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fo089m92g9ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1427">
+      <c r="A1427" t="inlineStr">
+        <is>
+          <t>1m9znek</t>
+        </is>
+      </c>
+      <c r="B1427" t="inlineStr">
+        <is>
+          <t>Nails I got in 2022 🩵🖤</t>
+        </is>
+      </c>
+      <c r="C1427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9znek</t>
+        </is>
+      </c>
+    </row>
+    <row r="1428">
+      <c r="A1428" t="inlineStr">
+        <is>
+          <t>1m9zcb0</t>
+        </is>
+      </c>
+      <c r="B1428" t="inlineStr">
+        <is>
+          <t>My last set for a while</t>
+        </is>
+      </c>
+      <c r="C1428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9zcb0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1429">
+      <c r="A1429" t="inlineStr">
+        <is>
+          <t>1m9z11z</t>
+        </is>
+      </c>
+      <c r="B1429" t="inlineStr">
+        <is>
+          <t>Natural nails ✨</t>
+        </is>
+      </c>
+      <c r="C1429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9z11z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1430">
+      <c r="A1430" t="inlineStr">
+        <is>
+          <t>1m9yqfa</t>
+        </is>
+      </c>
+      <c r="B1430" t="inlineStr">
+        <is>
+          <t>A gel manicure I did on myself the other day!</t>
+        </is>
+      </c>
+      <c r="C1430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9yqfa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1431">
+      <c r="A1431" t="inlineStr">
+        <is>
+          <t>1m9ypbz</t>
+        </is>
+      </c>
+      <c r="B1431" t="inlineStr">
+        <is>
+          <t>Pearl press on set</t>
+        </is>
+      </c>
+      <c r="C1431" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/f34e1wi449ff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1432">
+      <c r="A1432" t="inlineStr">
+        <is>
+          <t>1m9y9zn</t>
+        </is>
+      </c>
+      <c r="B1432" t="inlineStr">
+        <is>
+          <t>Can't text back, too busy admiring my claws</t>
+        </is>
+      </c>
+      <c r="C1432" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ebk6aj0419ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1433">
+      <c r="A1433" t="inlineStr">
+        <is>
+          <t>1m9y1ak</t>
+        </is>
+      </c>
+      <c r="B1433" t="inlineStr">
+        <is>
+          <t>Que uñas creen que me debería hacer para una fiesta si mi vestido es verde olivo?</t>
+        </is>
+      </c>
+      <c r="C1433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m9y1ak/que_uñas_creen_que_me_debería_hacer_para_una/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1434">
+      <c r="A1434" t="inlineStr">
+        <is>
+          <t>1m9xz1u</t>
+        </is>
+      </c>
+      <c r="B1434" t="inlineStr">
+        <is>
+          <t>I love cat eye look 🤩</t>
+        </is>
+      </c>
+      <c r="C1434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9xz1u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1435">
+      <c r="A1435" t="inlineStr">
+        <is>
+          <t>1m9xuzs</t>
+        </is>
+      </c>
+      <c r="B1435" t="inlineStr">
+        <is>
+          <t>It’s fish! (In my best Lilo voice)</t>
+        </is>
+      </c>
+      <c r="C1435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9xuzs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1436">
+      <c r="A1436" t="inlineStr">
+        <is>
+          <t>1m9xp66</t>
+        </is>
+      </c>
+      <c r="B1436" t="inlineStr">
+        <is>
+          <t>i did them myself :D</t>
+        </is>
+      </c>
+      <c r="C1436" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e7x5q18xw8ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1437">
+      <c r="A1437" t="inlineStr">
+        <is>
+          <t>1m9qxmv</t>
+        </is>
+      </c>
+      <c r="B1437" t="inlineStr">
+        <is>
+          <t>finding press ons</t>
+        </is>
+      </c>
+      <c r="C1437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9qxmv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1438">
+      <c r="A1438" t="inlineStr">
+        <is>
+          <t>1m9spx9</t>
+        </is>
+      </c>
+      <c r="B1438" t="inlineStr">
+        <is>
+          <t>How to avoid this</t>
+        </is>
+      </c>
+      <c r="C1438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9spx9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1439">
+      <c r="A1439" t="inlineStr">
+        <is>
+          <t>1m9wbge</t>
+        </is>
+      </c>
+      <c r="B1439" t="inlineStr">
+        <is>
+          <t>Sick nails 🖤🤘🎱</t>
+        </is>
+      </c>
+      <c r="C1439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9wbge</t>
+        </is>
+      </c>
+    </row>
+    <row r="1440">
+      <c r="A1440" t="inlineStr">
+        <is>
+          <t>1m9wyb4</t>
+        </is>
+      </c>
+      <c r="B1440" t="inlineStr">
+        <is>
+          <t>little tiny bows 🎀</t>
+        </is>
+      </c>
+      <c r="C1440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9wyb4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1441">
+      <c r="A1441" t="inlineStr">
+        <is>
+          <t>1m9wucj</t>
+        </is>
+      </c>
+      <c r="B1441" t="inlineStr">
+        <is>
+          <t>Another set of simple yet elegant nails</t>
+        </is>
+      </c>
+      <c r="C1441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9wucj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1442">
+      <c r="A1442" t="inlineStr">
+        <is>
+          <t>1m9wm9f</t>
+        </is>
+      </c>
+      <c r="B1442" t="inlineStr">
+        <is>
+          <t>Glittery pink 🩷</t>
+        </is>
+      </c>
+      <c r="C1442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9wm9f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1443">
+      <c r="A1443" t="inlineStr">
+        <is>
+          <t>1m9wjab</t>
+        </is>
+      </c>
+      <c r="B1443" t="inlineStr">
+        <is>
+          <t>Found my forever nail tech!</t>
+        </is>
+      </c>
+      <c r="C1443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9wjab</t>
+        </is>
+      </c>
+    </row>
+    <row r="1444">
+      <c r="A1444" t="inlineStr">
+        <is>
+          <t>1m9wi52</t>
+        </is>
+      </c>
+      <c r="B1444" t="inlineStr">
+        <is>
+          <t>My attempt at a new trend.</t>
+        </is>
+      </c>
+      <c r="C1444" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/84xdf96ao8ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1445">
+      <c r="A1445" t="inlineStr">
+        <is>
+          <t>1m9w85u</t>
+        </is>
+      </c>
+      <c r="B1445" t="inlineStr">
+        <is>
+          <t>Highlights of my best nails 💕</t>
+        </is>
+      </c>
+      <c r="C1445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9w85u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1446">
+      <c r="A1446" t="inlineStr">
+        <is>
+          <t>1m9vqft</t>
+        </is>
+      </c>
+      <c r="B1446" t="inlineStr">
+        <is>
+          <t>Glittery blue!</t>
+        </is>
+      </c>
+      <c r="C1446" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cmic5gzni8ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1447">
+      <c r="A1447" t="inlineStr">
+        <is>
+          <t>1m9vmxu</t>
+        </is>
+      </c>
+      <c r="B1447" t="inlineStr">
+        <is>
+          <t>Beach trip ready!</t>
+        </is>
+      </c>
+      <c r="C1447" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gdpbjljyh8ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1448">
+      <c r="A1448" t="inlineStr">
+        <is>
+          <t>1maguoc</t>
+        </is>
+      </c>
+      <c r="B1448" t="inlineStr">
+        <is>
+          <t>appreciate the review pics 😂</t>
+        </is>
+      </c>
+      <c r="C1448" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rldo32c6jdff1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1449">
+      <c r="A1449" t="inlineStr">
+        <is>
+          <t>1mag24s</t>
+        </is>
+      </c>
+      <c r="B1449" t="inlineStr">
+        <is>
+          <t>Uneven white part of nail that won’t reattach to the toe?</t>
+        </is>
+      </c>
+      <c r="C1449" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oh18sb9wadff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1450">
+      <c r="A1450" t="inlineStr">
+        <is>
+          <t>1mafb9d</t>
+        </is>
+      </c>
+      <c r="B1450" t="inlineStr">
+        <is>
+          <t>Moonkitty</t>
+        </is>
+      </c>
+      <c r="C1450" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c0n8s07m2dff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1451">
+      <c r="A1451" t="inlineStr">
+        <is>
+          <t>1maf0t5</t>
+        </is>
+      </c>
+      <c r="B1451" t="inlineStr">
+        <is>
+          <t>First gel polish attempt</t>
+        </is>
+      </c>
+      <c r="C1451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1maf0t5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1452">
+      <c r="A1452" t="inlineStr">
+        <is>
+          <t>1maekvw</t>
+        </is>
+      </c>
+      <c r="B1452" t="inlineStr">
+        <is>
+          <t>my nails + my gf’s! 💕</t>
+        </is>
+      </c>
+      <c r="C1452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1maekvw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1453">
+      <c r="A1453" t="inlineStr">
+        <is>
+          <t>1madbws</t>
+        </is>
+      </c>
+      <c r="B1453" t="inlineStr">
+        <is>
+          <t>Lurid A Formidable Opponent</t>
+        </is>
+      </c>
+      <c r="C1453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1madbws</t>
+        </is>
+      </c>
+    </row>
+    <row r="1454">
+      <c r="A1454" t="inlineStr">
+        <is>
+          <t>1mad1if</t>
+        </is>
+      </c>
+      <c r="B1454" t="inlineStr">
+        <is>
+          <t>Trying layering to make Curiosity's Prey more fun. Photos of the process at the end!</t>
+        </is>
+      </c>
+      <c r="C1454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mad1if</t>
+        </is>
+      </c>
+    </row>
+    <row r="1455">
+      <c r="A1455" t="inlineStr">
+        <is>
+          <t>1macmv6</t>
+        </is>
+      </c>
+      <c r="B1455" t="inlineStr">
+        <is>
+          <t>Oxblood and leopard print</t>
+        </is>
+      </c>
+      <c r="C1455" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ja2d37gacff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1456">
+      <c r="A1456" t="inlineStr">
+        <is>
+          <t>1macavg</t>
+        </is>
+      </c>
+      <c r="B1456" t="inlineStr">
+        <is>
+          <t>A little late to the party but here’s the spinner I made</t>
+        </is>
+      </c>
+      <c r="C1456" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nmo9coh57cff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1457">
+      <c r="A1457" t="inlineStr">
+        <is>
+          <t>1mabt7p</t>
+        </is>
+      </c>
+      <c r="B1457" t="inlineStr">
+        <is>
+          <t>Finally happy with my set up</t>
+        </is>
+      </c>
+      <c r="C1457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mabt7p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1458">
+      <c r="A1458" t="inlineStr">
+        <is>
+          <t>1maaui4</t>
+        </is>
+      </c>
+      <c r="B1458" t="inlineStr">
+        <is>
+          <t>These are the longest nails I've ever had.</t>
+        </is>
+      </c>
+      <c r="C1458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1maaui4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1459">
+      <c r="A1459" t="inlineStr">
+        <is>
+          <t>1maarkk</t>
+        </is>
+      </c>
+      <c r="B1459" t="inlineStr">
+        <is>
+          <t>Trying out colors I don’t usually wear</t>
+        </is>
+      </c>
+      <c r="C1459" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nncj63gasbff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1460">
+      <c r="A1460" t="inlineStr">
+        <is>
+          <t>1maa2sk</t>
+        </is>
+      </c>
+      <c r="B1460" t="inlineStr">
+        <is>
+          <t>what is a color that makes you look dead?</t>
+        </is>
+      </c>
+      <c r="C1460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1maa2sk/what_is_a_color_that_makes_you_look_dead/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1461">
+      <c r="A1461" t="inlineStr">
+        <is>
+          <t>1ma9yla</t>
+        </is>
+      </c>
+      <c r="B1461" t="inlineStr">
+        <is>
+          <t>my nails split layer by layer(circled). i’ve never seen anyone else with this issue on their nails in real life. how do i prevent this?</t>
+        </is>
+      </c>
+      <c r="C1461" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/86kbt3iclbff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1462">
+      <c r="A1462" t="inlineStr">
+        <is>
+          <t>1ma9a3z</t>
+        </is>
+      </c>
+      <c r="B1462" t="inlineStr">
+        <is>
+          <t>Painting the sky</t>
+        </is>
+      </c>
+      <c r="C1462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ma9a3z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1463">
+      <c r="A1463" t="inlineStr">
+        <is>
+          <t>1ma99hy</t>
+        </is>
+      </c>
+      <c r="B1463" t="inlineStr">
+        <is>
+          <t>Rainbow of nail polish bottles</t>
+        </is>
+      </c>
+      <c r="C1463" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qr1blszyebff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1464">
+      <c r="A1464" t="inlineStr">
+        <is>
+          <t>1ma96ts</t>
+        </is>
+      </c>
+      <c r="B1464" t="inlineStr">
+        <is>
+          <t>Alchemy Lacquers - Emotional Support Taco</t>
+        </is>
+      </c>
+      <c r="C1464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ma96ts</t>
+        </is>
+      </c>
+    </row>
+    <row r="1465">
+      <c r="A1465" t="inlineStr">
+        <is>
+          <t>1ma8lto</t>
+        </is>
+      </c>
+      <c r="B1465" t="inlineStr">
+        <is>
+          <t>Fidget spinner day 2 nails, ILNP flip side</t>
+        </is>
+      </c>
+      <c r="C1465" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lpj74gq19bff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1466">
+      <c r="A1466" t="inlineStr">
+        <is>
+          <t>1ma89nr</t>
+        </is>
+      </c>
+      <c r="B1466" t="inlineStr">
+        <is>
+          <t>💙4️⃣Fantastic Four4️⃣💙</t>
+        </is>
+      </c>
+      <c r="C1466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ma89nr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1467">
+      <c r="A1467" t="inlineStr">
+        <is>
+          <t>1ma7k3i</t>
+        </is>
+      </c>
+      <c r="B1467" t="inlineStr">
+        <is>
+          <t>Favorite Muted Mooncat polishes?</t>
+        </is>
+      </c>
+      <c r="C1467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ma7k3i/favorite_muted_mooncat_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1468">
+      <c r="A1468" t="inlineStr">
+        <is>
+          <t>1ma7ijj</t>
+        </is>
+      </c>
+      <c r="B1468" t="inlineStr">
+        <is>
+          <t>First time trying ILNP 🌸💜</t>
+        </is>
+      </c>
+      <c r="C1468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ma7ijj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1469">
+      <c r="A1469" t="inlineStr">
+        <is>
+          <t>1ma7ho2</t>
+        </is>
+      </c>
+      <c r="B1469" t="inlineStr">
+        <is>
+          <t>First time flowers 🌼</t>
+        </is>
+      </c>
+      <c r="C1469" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3dt7d7nbzaff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1470">
+      <c r="A1470" t="inlineStr">
+        <is>
+          <t>1ma7fay</t>
+        </is>
+      </c>
+      <c r="B1470" t="inlineStr">
+        <is>
+          <t>Black Swan 🦢🖤</t>
+        </is>
+      </c>
+      <c r="C1470" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/78x6mr8myaff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1471">
+      <c r="A1471" t="inlineStr">
+        <is>
+          <t>1ma79pi</t>
+        </is>
+      </c>
+      <c r="B1471" t="inlineStr">
+        <is>
+          <t>New nailsss🩵</t>
+        </is>
+      </c>
+      <c r="C1471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ma79pi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1472">
+      <c r="A1472" t="inlineStr">
+        <is>
+          <t>1ma6c6r</t>
+        </is>
+      </c>
+      <c r="B1472" t="inlineStr">
+        <is>
+          <t>first time trying nail art on myself!</t>
+        </is>
+      </c>
+      <c r="C1472" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ggrwa4szoaff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1473">
+      <c r="A1473" t="inlineStr">
+        <is>
+          <t>1ma69nb</t>
+        </is>
+      </c>
+      <c r="B1473" t="inlineStr">
+        <is>
+          <t>Feel like traveling!</t>
+        </is>
+      </c>
+      <c r="C1473" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bhzciq34paff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1474">
+      <c r="A1474" t="inlineStr">
+        <is>
+          <t>1ma68fx</t>
+        </is>
+      </c>
+      <c r="B1474" t="inlineStr">
+        <is>
+          <t>How to make cuticles look better?</t>
+        </is>
+      </c>
+      <c r="C1474" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8vi2amhtoaff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1475">
+      <c r="A1475" t="inlineStr">
+        <is>
+          <t>1ma65g7</t>
+        </is>
+      </c>
+      <c r="B1475" t="inlineStr">
+        <is>
+          <t>jewel beetle is that girl! 🪲💘</t>
+        </is>
+      </c>
+      <c r="C1475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ma65g7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1476">
+      <c r="A1476" t="inlineStr">
+        <is>
+          <t>1ma658v</t>
+        </is>
+      </c>
+      <c r="B1476" t="inlineStr">
+        <is>
+          <t>Nail Health Issues</t>
+        </is>
+      </c>
+      <c r="C1476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ma658v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1477">
+      <c r="A1477" t="inlineStr">
+        <is>
+          <t>1ma64ol</t>
+        </is>
+      </c>
+      <c r="B1477" t="inlineStr">
+        <is>
+          <t>Duped myself - Flip Side vs Purple Party Monster</t>
+        </is>
+      </c>
+      <c r="C1477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ma64ol</t>
+        </is>
+      </c>
+    </row>
+    <row r="1478">
+      <c r="A1478" t="inlineStr">
+        <is>
+          <t>1ma5yaq</t>
+        </is>
+      </c>
+      <c r="B1478" t="inlineStr">
+        <is>
+          <t>saw a question about pure ice…</t>
+        </is>
+      </c>
+      <c r="C1478" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ne1vtjbjmaff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1479">
+      <c r="A1479" t="inlineStr">
+        <is>
+          <t>1ma5xie</t>
+        </is>
+      </c>
+      <c r="B1479" t="inlineStr">
+        <is>
+          <t>What is the trick to sponge gradients?</t>
+        </is>
+      </c>
+      <c r="C1479" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ma5xie</t>
+        </is>
+      </c>
+    </row>
+    <row r="1480">
+      <c r="A1480" t="inlineStr">
+        <is>
+          <t>1ma5uzj</t>
+        </is>
+      </c>
+      <c r="B1480" t="inlineStr">
+        <is>
+          <t>Pomegranate seeds from mooncat is so beautiful</t>
+        </is>
+      </c>
+      <c r="C1480" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/urwmslfulaff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1481">
+      <c r="A1481" t="inlineStr">
+        <is>
+          <t>1ma5jpe</t>
+        </is>
+      </c>
+      <c r="B1481" t="inlineStr">
+        <is>
+          <t>Does anyone have Leaf Of Faith (KBShimmer) / Fierce Forces (Emily de Molly) and/or I Got A Crush On You (KBShimmer) / Luminous Forces (Emily de Molly)? How these polishes compare?</t>
+        </is>
+      </c>
+      <c r="C1481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ma5jpe/does_anyone_have_leaf_of_faith_kbshimmer_fierce/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1482">
+      <c r="A1482" t="inlineStr">
+        <is>
+          <t>1ma1aen</t>
+        </is>
+      </c>
+      <c r="B1482" t="inlineStr">
+        <is>
+          <t>Jelly skittle! 🍬</t>
+        </is>
+      </c>
+      <c r="C1482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ma1aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="1483">
+      <c r="A1483" t="inlineStr">
+        <is>
+          <t>1ma3zp8</t>
+        </is>
+      </c>
+      <c r="B1483" t="inlineStr">
+        <is>
+          <t>Which of these are fake because the font doesn’t match help</t>
+        </is>
+      </c>
+      <c r="C1483" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/41m9vpdt6aff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1484">
+      <c r="A1484" t="inlineStr">
+        <is>
+          <t>1ma55nb</t>
+        </is>
+      </c>
+      <c r="B1484" t="inlineStr">
+        <is>
+          <t>Sticky base coat sold in-store UK?</t>
+        </is>
+      </c>
+      <c r="C1484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ma55nb/sticky_base_coat_sold_instore_uk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1485">
+      <c r="A1485" t="inlineStr">
+        <is>
+          <t>1ma53m2</t>
+        </is>
+      </c>
+      <c r="B1485" t="inlineStr">
+        <is>
+          <t>💅</t>
+        </is>
+      </c>
+      <c r="C1485" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/huiywagyfaff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1486">
+      <c r="A1486" t="inlineStr">
+        <is>
+          <t>1ma4v0f</t>
+        </is>
+      </c>
+      <c r="B1486" t="inlineStr">
+        <is>
+          <t>What shape looks better?</t>
+        </is>
+      </c>
+      <c r="C1486" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ma4v0f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1487">
+      <c r="A1487" t="inlineStr">
+        <is>
+          <t>1ma4coh</t>
+        </is>
+      </c>
+      <c r="B1487" t="inlineStr">
+        <is>
+          <t>Rum Ham is a hit</t>
+        </is>
+      </c>
+      <c r="C1487" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2cxs3c16aaff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1488">
+      <c r="A1488" t="inlineStr">
+        <is>
+          <t>1ma41vf</t>
+        </is>
+      </c>
+      <c r="B1488" t="inlineStr">
+        <is>
+          <t>Easy magnet setup for glass bead effect?</t>
+        </is>
+      </c>
+      <c r="C1488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ma41vf/easy_magnet_setup_for_glass_bead_effect/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1489">
+      <c r="A1489" t="inlineStr">
+        <is>
+          <t>1ma3w9b</t>
+        </is>
+      </c>
+      <c r="B1489" t="inlineStr">
+        <is>
+          <t>Rogue Lacquer faves and topper opinions?</t>
+        </is>
+      </c>
+      <c r="C1489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ma3w9b/rogue_lacquer_faves_and_topper_opinions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1490">
+      <c r="A1490" t="inlineStr">
+        <is>
+          <t>1ma3t3q</t>
+        </is>
+      </c>
+      <c r="B1490" t="inlineStr">
+        <is>
+          <t>Sparkling Blush</t>
+        </is>
+      </c>
+      <c r="C1490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ma3t3q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1491">
+      <c r="A1491" t="inlineStr">
+        <is>
+          <t>1ma3nlv</t>
+        </is>
+      </c>
+      <c r="B1491" t="inlineStr">
+        <is>
+          <t>Plant Aunt over F*ck Kale</t>
+        </is>
+      </c>
+      <c r="C1491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ma3nlv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1492">
+      <c r="A1492" t="inlineStr">
+        <is>
+          <t>1ma39ej</t>
+        </is>
+      </c>
+      <c r="B1492" t="inlineStr">
+        <is>
+          <t>I’m so damn proud of this mani, idk how I’ll ever top it! 🏳️‍🌈</t>
+        </is>
+      </c>
+      <c r="C1492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ma39ej</t>
+        </is>
+      </c>
+    </row>
+    <row r="1493">
+      <c r="A1493" t="inlineStr">
+        <is>
+          <t>1ma2s8w</t>
+        </is>
+      </c>
+      <c r="B1493" t="inlineStr">
+        <is>
+          <t>Milky Wave🩵🌌</t>
+        </is>
+      </c>
+      <c r="C1493" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/d22nhlu7y9ff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1494">
+      <c r="A1494" t="inlineStr">
+        <is>
+          <t>1ma2ffu</t>
+        </is>
+      </c>
+      <c r="B1494" t="inlineStr">
+        <is>
+          <t>Absolutely magical 🌈 ✨ 💖</t>
+        </is>
+      </c>
+      <c r="C1494" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ma2ffu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1495">
+      <c r="A1495" t="inlineStr">
+        <is>
+          <t>1ma2d7x</t>
+        </is>
+      </c>
+      <c r="B1495" t="inlineStr">
+        <is>
+          <t>I never expected this polish to be this beautiful</t>
+        </is>
+      </c>
+      <c r="C1495" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/01yeuidtu9ff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1496">
+      <c r="A1496" t="inlineStr">
+        <is>
+          <t>1ma1zlr</t>
+        </is>
+      </c>
+      <c r="B1496" t="inlineStr">
+        <is>
+          <t>Looking for polishes to dupe an old favourite!</t>
+        </is>
+      </c>
+      <c r="C1496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ma1zlr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1497">
+      <c r="A1497" t="inlineStr">
+        <is>
+          <t>1ma1n42</t>
+        </is>
+      </c>
+      <c r="B1497" t="inlineStr">
+        <is>
+          <t>So excited with my new flakes!</t>
+        </is>
+      </c>
+      <c r="C1497" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ma1n42</t>
+        </is>
+      </c>
+    </row>
+    <row r="1498">
+      <c r="A1498" t="inlineStr">
+        <is>
+          <t>1ma1ia5</t>
+        </is>
+      </c>
+      <c r="B1498" t="inlineStr">
+        <is>
+          <t>What are some brands that do videogame-inspired or themed collections?</t>
+        </is>
+      </c>
+      <c r="C1498" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ma1ia5/what_are_some_brands_that_do_videogameinspired_or/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1499">
+      <c r="A1499" t="inlineStr">
+        <is>
+          <t>1ma14kv</t>
+        </is>
+      </c>
+      <c r="B1499" t="inlineStr">
+        <is>
+          <t>Telling me I need to stop buying polishes, then asking to use said collection to paint jewelry... WTH! 🤷‍♀️</t>
+        </is>
+      </c>
+      <c r="C1499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ma14kv/telling_me_i_need_to_stop_buying_polishes_then/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1500">
+      <c r="A1500" t="inlineStr">
+        <is>
+          <t>1ma0zxb</t>
+        </is>
+      </c>
+      <c r="B1500" t="inlineStr">
+        <is>
+          <t>🌷 Flower Child 🌺</t>
+        </is>
+      </c>
+      <c r="C1500" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ma0zxb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1501">
+      <c r="A1501" t="inlineStr">
+        <is>
+          <t>1ma0s27</t>
+        </is>
+      </c>
+      <c r="B1501" t="inlineStr">
+        <is>
+          <t>POV: This nail breaks. You cutting them all down or using it to try doing lipstick shape?</t>
+        </is>
+      </c>
+      <c r="C1501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ma0s27</t>
+        </is>
+      </c>
+    </row>
+    <row r="1502">
+      <c r="A1502" t="inlineStr">
+        <is>
+          <t>1m9zxqo</t>
+        </is>
+      </c>
+      <c r="B1502" t="inlineStr">
+        <is>
+          <t>VS top coat is tinted?</t>
+        </is>
+      </c>
+      <c r="C1502" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9zxqo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1503">
+      <c r="A1503" t="inlineStr">
+        <is>
+          <t>1m9ztqo</t>
+        </is>
+      </c>
+      <c r="B1503" t="inlineStr">
+        <is>
+          <t>Collection show-off as I go on a no-buy 💅</t>
+        </is>
+      </c>
+      <c r="C1503" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9ztqo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1504">
+      <c r="A1504" t="inlineStr">
+        <is>
+          <t>1m9zozm</t>
+        </is>
+      </c>
+      <c r="B1504" t="inlineStr">
+        <is>
+          <t>Guess who? 🌌🌌🌌</t>
+        </is>
+      </c>
+      <c r="C1504" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9zozm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1505">
+      <c r="A1505" t="inlineStr">
+        <is>
+          <t>1m9znrh</t>
+        </is>
+      </c>
+      <c r="B1505" t="inlineStr">
+        <is>
+          <t>Help my nails are trapped in a computer 😭</t>
+        </is>
+      </c>
+      <c r="C1505" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9znrh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1506">
+      <c r="A1506" t="inlineStr">
+        <is>
+          <t>1m9zmt2</t>
+        </is>
+      </c>
+      <c r="B1506" t="inlineStr">
+        <is>
+          <t>Nail Break or Start of Something Better</t>
+        </is>
+      </c>
+      <c r="C1506" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9zmt2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1507">
+      <c r="A1507" t="inlineStr">
+        <is>
+          <t>1m9zhm0</t>
+        </is>
+      </c>
+      <c r="B1507" t="inlineStr">
+        <is>
+          <t>Reminding myself that summer doesn't last forever ❄️</t>
+        </is>
+      </c>
+      <c r="C1507" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9zhm0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1508">
+      <c r="A1508" t="inlineStr">
+        <is>
+          <t>1m9z2vk</t>
+        </is>
+      </c>
+      <c r="B1508" t="inlineStr">
+        <is>
+          <t>New Clionadh collection!</t>
+        </is>
+      </c>
+      <c r="C1508" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9z2vk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1509">
+      <c r="A1509" t="inlineStr">
+        <is>
+          <t>1m9yz55</t>
+        </is>
+      </c>
+      <c r="B1509" t="inlineStr">
+        <is>
+          <t>Oxblood reds only</t>
+        </is>
+      </c>
+      <c r="C1509" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9yz55</t>
+        </is>
+      </c>
+    </row>
+    <row r="1510">
+      <c r="A1510" t="inlineStr">
+        <is>
+          <t>1m9ye89</t>
+        </is>
+      </c>
+      <c r="B1510" t="inlineStr">
+        <is>
+          <t>I didn't have high hopes... I couldn't have been more wrong ㅣ WakeMake "Glowy Silk"</t>
+        </is>
+      </c>
+      <c r="C1510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9ye89</t>
+        </is>
+      </c>
+    </row>
+    <row r="1511">
+      <c r="A1511" t="inlineStr">
+        <is>
+          <t>1m9y5ze</t>
+        </is>
+      </c>
+      <c r="B1511" t="inlineStr">
+        <is>
+          <t>Hunger Games Polish</t>
+        </is>
+      </c>
+      <c r="C1511" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n9iang2a09ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1512">
+      <c r="A1512" t="inlineStr">
+        <is>
+          <t>1m9y5as</t>
+        </is>
+      </c>
+      <c r="B1512" t="inlineStr">
+        <is>
+          <t>Natural nails + Scarlet Red</t>
+        </is>
+      </c>
+      <c r="C1512" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9y5as</t>
+        </is>
+      </c>
+    </row>
+    <row r="1513">
+      <c r="A1513" t="inlineStr">
+        <is>
+          <t>1m9xxt0</t>
+        </is>
+      </c>
+      <c r="B1513" t="inlineStr">
+        <is>
+          <t>brands/ lines with this kind of brush?</t>
+        </is>
+      </c>
+      <c r="C1513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m9xxt0/brands_lines_with_this_kind_of_brush/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1514">
+      <c r="A1514" t="inlineStr">
+        <is>
+          <t>1m9xgti</t>
+        </is>
+      </c>
+      <c r="B1514" t="inlineStr">
+        <is>
+          <t>Tropical island breeze, all of nature wild and free</t>
+        </is>
+      </c>
+      <c r="C1514" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9xgti</t>
+        </is>
+      </c>
+    </row>
+    <row r="1515">
+      <c r="A1515" t="inlineStr">
+        <is>
+          <t>1m9x29y</t>
+        </is>
+      </c>
+      <c r="B1515" t="inlineStr">
+        <is>
+          <t>Looking for an iridescent polish that looks like these photos.</t>
+        </is>
+      </c>
+      <c r="C1515" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/36ms2cr9s8ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1516">
+      <c r="A1516" t="inlineStr">
+        <is>
+          <t>1m9x11i</t>
+        </is>
+      </c>
+      <c r="B1516" t="inlineStr">
+        <is>
+          <t>A Tale of 2 Disco Balls</t>
+        </is>
+      </c>
+      <c r="C1516" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8wrmny11s8ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1517">
+      <c r="A1517" t="inlineStr">
+        <is>
+          <t>1m9ww4u</t>
+        </is>
+      </c>
+      <c r="B1517" t="inlineStr">
+        <is>
+          <t>I was worried it would look bad on my skin but I love it</t>
+        </is>
+      </c>
+      <c r="C1517" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xg776sz3r8ff1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1518">
+      <c r="A1518" t="inlineStr">
+        <is>
+          <t>1m9wazo</t>
+        </is>
+      </c>
+      <c r="B1518" t="inlineStr">
+        <is>
+          <t>Convince me to buy your favorite polish in one photo</t>
+        </is>
+      </c>
+      <c r="C1518" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m9wazo/convince_me_to_buy_your_favorite_polish_in_one/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1519">
+      <c r="A1519" t="inlineStr">
+        <is>
+          <t>1m9w41p</t>
+        </is>
+      </c>
+      <c r="B1519" t="inlineStr">
+        <is>
+          <t>Layering polish, who would've thunk it?</t>
+        </is>
+      </c>
+      <c r="C1519" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m9w41p/layering_polish_who_wouldve_thunk_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1520">
+      <c r="A1520" t="inlineStr">
+        <is>
+          <t>1m9vkua</t>
+        </is>
+      </c>
+      <c r="B1520" t="inlineStr">
+        <is>
+          <t>Ring Inspo Mani!</t>
+        </is>
+      </c>
+      <c r="C1520" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/awimYDY</t>
+        </is>
+      </c>
+    </row>
+    <row r="1521">
+      <c r="A1521" t="inlineStr">
+        <is>
+          <t>1m9upm3</t>
+        </is>
+      </c>
+      <c r="B1521" t="inlineStr">
+        <is>
+          <t>It’s so shifty 😍</t>
+        </is>
+      </c>
+      <c r="C1521" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9upm3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1522">
+      <c r="A1522" t="inlineStr">
+        <is>
+          <t>1m9ultj</t>
+        </is>
+      </c>
+      <c r="B1522" t="inlineStr">
+        <is>
+          <t>Serpents of Eden</t>
+        </is>
+      </c>
+      <c r="C1522" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9ultj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1523">
+      <c r="A1523" t="inlineStr">
+        <is>
+          <t>1m9ub8d</t>
+        </is>
+      </c>
+      <c r="B1523" t="inlineStr">
+        <is>
+          <t>Strong Independent Woman Who Absolutely Needs A Mani</t>
+        </is>
+      </c>
+      <c r="C1523" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/62v3sffz78ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1524">
+      <c r="A1524" t="inlineStr">
+        <is>
+          <t>1m9tzgr</t>
+        </is>
+      </c>
+      <c r="B1524" t="inlineStr">
+        <is>
+          <t>Sassy Sauce 🫶</t>
+        </is>
+      </c>
+      <c r="C1524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9tzgr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1525">
+      <c r="A1525" t="inlineStr">
+        <is>
+          <t>1m9qk1a</t>
+        </is>
+      </c>
+      <c r="B1525" t="inlineStr">
+        <is>
+          <t>i’m very happy! 7 days without any chipping</t>
+        </is>
+      </c>
+      <c r="C1525" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9qk1a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1526">
+      <c r="A1526" t="inlineStr">
+        <is>
+          <t>1m9qfzi</t>
+        </is>
+      </c>
+      <c r="B1526" t="inlineStr">
+        <is>
+          <t>Took off builder gel after 2.5 years!</t>
+        </is>
+      </c>
+      <c r="C1526" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1hwyyio297ff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1527">
+      <c r="A1527" t="inlineStr">
+        <is>
+          <t>1m9pk0t</t>
+        </is>
+      </c>
+      <c r="B1527" t="inlineStr">
+        <is>
+          <t>Nails are ridged, break and split</t>
+        </is>
+      </c>
+      <c r="C1527" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m9pk0t/nails_are_ridged_break_and_split/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1528">
+      <c r="A1528" t="inlineStr">
+        <is>
+          <t>1m9p9gs</t>
+        </is>
+      </c>
+      <c r="B1528" t="inlineStr">
+        <is>
+          <t>First time trying nail art! How did I do?</t>
+        </is>
+      </c>
+      <c r="C1528" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9p9gs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1529">
+      <c r="A1529" t="inlineStr">
+        <is>
+          <t>1m9oz3n</t>
+        </is>
+      </c>
+      <c r="B1529" t="inlineStr">
+        <is>
+          <t>The Dichotomy of Cat Swatches</t>
+        </is>
+      </c>
+      <c r="C1529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9oz3n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1530">
+      <c r="A1530" t="inlineStr">
+        <is>
+          <t>1m9okce</t>
+        </is>
+      </c>
+      <c r="B1530" t="inlineStr">
+        <is>
+          <t>Phoenix Indie: As the World Falls Down</t>
+        </is>
+      </c>
+      <c r="C1530" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zrb2reuqm6ff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1531">
+      <c r="A1531" t="inlineStr">
+        <is>
+          <t>1madpo2</t>
+        </is>
+      </c>
+      <c r="B1531" t="inlineStr">
+        <is>
+          <t>Shipping in summer - will it ruin gel polish?</t>
+        </is>
+      </c>
+      <c r="C1531" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1madpo2/shipping_in_summer_will_it_ruin_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1532">
+      <c r="A1532" t="inlineStr">
+        <is>
+          <t>1madlr2</t>
+        </is>
+      </c>
+      <c r="B1532" t="inlineStr">
+        <is>
+          <t>first time doing nails!</t>
+        </is>
+      </c>
+      <c r="C1532" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1madlr2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1533">
+      <c r="A1533" t="inlineStr">
+        <is>
+          <t>1ma9rxc</t>
+        </is>
+      </c>
+      <c r="B1533" t="inlineStr">
+        <is>
+          <t>Dinosaur nails!!</t>
+        </is>
+      </c>
+      <c r="C1533" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j46omwzkjbff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1534">
+      <c r="A1534" t="inlineStr">
+        <is>
+          <t>1ma9p2d</t>
+        </is>
+      </c>
+      <c r="B1534" t="inlineStr">
+        <is>
+          <t>I think tortoise shell print might have me in a chokehold now 😍</t>
+        </is>
+      </c>
+      <c r="C1534" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ma9p2d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1535">
+      <c r="A1535" t="inlineStr">
+        <is>
+          <t>1ma9ey3</t>
+        </is>
+      </c>
+      <c r="B1535" t="inlineStr">
+        <is>
+          <t>Alguien más ama el color rojo? ❤️</t>
+        </is>
+      </c>
+      <c r="C1535" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ma9ey3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1536">
+      <c r="A1536" t="inlineStr">
+        <is>
+          <t>1ma7tzy</t>
+        </is>
+      </c>
+      <c r="B1536" t="inlineStr">
+        <is>
+          <t>Hopped on the tik tok octopus nails trend🐙</t>
+        </is>
+      </c>
+      <c r="C1536" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3px8mgy82bff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1537">
+      <c r="A1537" t="inlineStr">
+        <is>
+          <t>1ma7he3</t>
+        </is>
+      </c>
+      <c r="B1537" t="inlineStr">
+        <is>
+          <t>Cute idea for nail art!</t>
+        </is>
+      </c>
+      <c r="C1537" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/reel/DMcLbHtR7QA/?igsh=cWZrNzJvcnpubXpz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1538">
+      <c r="A1538" t="inlineStr">
+        <is>
+          <t>1ma74vw</t>
+        </is>
+      </c>
+      <c r="B1538" t="inlineStr">
+        <is>
+          <t>🌟NEW Nail art for my chef lady 👩🏻‍🍳</t>
+        </is>
+      </c>
+      <c r="C1538" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ma74vw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1539">
+      <c r="A1539" t="inlineStr">
+        <is>
+          <t>1ma6ond</t>
+        </is>
+      </c>
+      <c r="B1539" t="inlineStr">
+        <is>
+          <t>Water &amp; Lava</t>
+        </is>
+      </c>
+      <c r="C1539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ma6ond</t>
+        </is>
+      </c>
+    </row>
+    <row r="1540">
+      <c r="A1540" t="inlineStr">
+        <is>
+          <t>1ma6jng</t>
+        </is>
+      </c>
+      <c r="B1540" t="inlineStr">
+        <is>
+          <t>This group taught me to stamp nails, so I am returning the favor with a tutorial of my own</t>
+        </is>
+      </c>
+      <c r="C1540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ma6jng</t>
+        </is>
+      </c>
+    </row>
+    <row r="1541">
+      <c r="A1541" t="inlineStr">
+        <is>
+          <t>1ma5rx3</t>
+        </is>
+      </c>
+      <c r="B1541" t="inlineStr">
+        <is>
+          <t>Green energy 💚</t>
+        </is>
+      </c>
+      <c r="C1541" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hby7aab6laff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1542">
+      <c r="A1542" t="inlineStr">
+        <is>
+          <t>1ma4omt</t>
+        </is>
+      </c>
+      <c r="B1542" t="inlineStr">
+        <is>
+          <t>Why does this happen</t>
+        </is>
+      </c>
+      <c r="C1542" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/26662o5pcaff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1543">
+      <c r="A1543" t="inlineStr">
+        <is>
+          <t>1ma3tz1</t>
+        </is>
+      </c>
+      <c r="B1543" t="inlineStr">
+        <is>
+          <t>Nail conditions reboot 🦠</t>
+        </is>
+      </c>
+      <c r="C1543" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w1ol8fk76aff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1544">
+      <c r="A1544" t="inlineStr">
+        <is>
+          <t>1ma3f5w</t>
+        </is>
+      </c>
+      <c r="B1544" t="inlineStr">
+        <is>
+          <t>Is it okay to do gel every day?</t>
+        </is>
+      </c>
+      <c r="C1544" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z3fqfbd33aff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1545">
+      <c r="A1545" t="inlineStr">
+        <is>
+          <t>1ma2bre</t>
+        </is>
+      </c>
+      <c r="B1545" t="inlineStr">
+        <is>
+          <t>Touch of summer on my thumbnail 🥰</t>
+        </is>
+      </c>
+      <c r="C1545" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/irsaebdsu9ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1546">
+      <c r="A1546" t="inlineStr">
+        <is>
+          <t>1ma28sh</t>
+        </is>
+      </c>
+      <c r="B1546" t="inlineStr">
+        <is>
+          <t>Nail_girl</t>
+        </is>
+      </c>
+      <c r="C1546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ma28sh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1547">
+      <c r="A1547" t="inlineStr">
+        <is>
+          <t>1ma0pr6</t>
+        </is>
+      </c>
+      <c r="B1547" t="inlineStr">
+        <is>
+          <t>Quartz set 💎 🩵</t>
+        </is>
+      </c>
+      <c r="C1547" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ma0pr6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1548">
+      <c r="A1548" t="inlineStr">
+        <is>
+          <t>1ma0isv</t>
+        </is>
+      </c>
+      <c r="B1548" t="inlineStr">
+        <is>
+          <t>First of 10 cityscape nails! Liking the new challenge!</t>
+        </is>
+      </c>
+      <c r="C1548" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/e65b6r7ng9ff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1549">
+      <c r="A1549" t="inlineStr">
+        <is>
+          <t>1m9yn0p</t>
+        </is>
+      </c>
+      <c r="B1549" t="inlineStr">
+        <is>
+          <t>Pretty and clean with some gold accents 🤌🏻 @sueznails</t>
+        </is>
+      </c>
+      <c r="C1549" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9yn0p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1550">
+      <c r="A1550" t="inlineStr">
+        <is>
+          <t>1m9yenn</t>
+        </is>
+      </c>
+      <c r="B1550" t="inlineStr">
+        <is>
+          <t>Who doesn’t love cheetah print?! Slayed by @sueznails @ @phillysnails</t>
+        </is>
+      </c>
+      <c r="C1550" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bu4rc4u129ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1551">
+      <c r="A1551" t="inlineStr">
+        <is>
+          <t>1m9xxo2</t>
+        </is>
+      </c>
+      <c r="B1551" t="inlineStr">
+        <is>
+          <t>Les gusta ? 🫣</t>
+        </is>
+      </c>
+      <c r="C1551" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a8hb6t1ny8ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1552">
+      <c r="A1552" t="inlineStr">
+        <is>
+          <t>1m9vrrl</t>
+        </is>
+      </c>
+      <c r="B1552" t="inlineStr">
+        <is>
+          <t>🐥💐🤍</t>
+        </is>
+      </c>
+      <c r="C1552" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q2ud6qzxi8ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1553">
+      <c r="A1553" t="inlineStr">
+        <is>
+          <t>1m9ud1h</t>
+        </is>
+      </c>
+      <c r="B1553" t="inlineStr">
+        <is>
+          <t>Made this set with so much love 🌸 Do you feel the summer vibes? 🤭</t>
+        </is>
+      </c>
+      <c r="C1553" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rva6cj8d88ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1554">
+      <c r="A1554" t="inlineStr">
+        <is>
+          <t>1m9paj9</t>
+        </is>
+      </c>
+      <c r="B1554" t="inlineStr">
+        <is>
+          <t>Dual shading from layering 🧜🏿‍♂️</t>
+        </is>
+      </c>
+      <c r="C1554" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3tpuqxfvv6ff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1555">
+      <c r="A1555" t="inlineStr">
+        <is>
+          <t>1m9ozgg</t>
+        </is>
+      </c>
+      <c r="B1555" t="inlineStr">
+        <is>
+          <t>Holiday nails 🌴☀️</t>
+        </is>
+      </c>
+      <c r="C1555" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/njgejj77s6ff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1556">
+      <c r="A1556" t="inlineStr">
+        <is>
+          <t>1m9o38e</t>
+        </is>
+      </c>
+      <c r="B1556" t="inlineStr">
+        <is>
+          <t>I feel like it wasn’t visible in the video</t>
+        </is>
+      </c>
+      <c r="C1556" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m9o38e</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>